<commit_message>
Edits to EFS_BOM and file structure fixes
</commit_message>
<xml_diff>
--- a/Purchasing/EFS_BOM.xlsx
+++ b/Purchasing/EFS_BOM.xlsx
@@ -78,9 +78,6 @@
   </si>
   <si>
     <t>3A</t>
-  </si>
-  <si>
-    <t>Rotating assembly:</t>
   </si>
   <si>
     <t>External Retaining Ring for 20mm Shaft Diameter</t>
@@ -252,9 +249,6 @@
   </si>
   <si>
     <t>6362K307</t>
-  </si>
-  <si>
-    <t>used as the initial seal</t>
   </si>
   <si>
     <t>Micro boring bar</t>
@@ -493,6 +487,12 @@
   <si>
     <t xml:space="preserve">pkg (25) Metric Type 316 Stainless Steel </t>
   </si>
+  <si>
+    <t>Rotating Assembly:</t>
+  </si>
+  <si>
+    <t>Used as the initial spec seal</t>
+  </si>
 </sst>
 </file>
 
@@ -505,7 +505,7 @@
     <numFmt numFmtId="166" formatCode="\$#,##0.00\ ;[Red]&quot;($&quot;#,##0.00\)"/>
     <numFmt numFmtId="167" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -609,8 +609,15 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="13"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -644,6 +651,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -734,7 +747,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -762,9 +775,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="8" fillId="6" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="167" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -789,9 +799,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -801,9 +808,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -812,9 +816,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -836,9 +837,6 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -882,38 +880,56 @@
     <xf numFmtId="0" fontId="13" fillId="6" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="7" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1268,8 +1284,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AVF73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13:O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1279,9 +1295,9 @@
     <col min="3" max="3" width="20.5703125" style="1" customWidth="1"/>
     <col min="4" max="4" width="15.28515625" style="1" customWidth="1"/>
     <col min="5" max="5" width="25.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="26.140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="25.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="9.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="21" style="1" customWidth="1"/>
+    <col min="7" max="7" width="20.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="1" customWidth="1"/>
     <col min="9" max="9" width="13.7109375" style="1" customWidth="1"/>
     <col min="10" max="13" width="3.5703125" style="1" customWidth="1"/>
     <col min="14" max="14" width="7" style="1" customWidth="1"/>
@@ -1291,7 +1307,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1254" s="2" customFormat="1" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="64" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
@@ -1313,19 +1329,19 @@
         <v>6</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
-      <c r="J1" s="61" t="s">
+      <c r="J1" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="61"/>
-      <c r="L1" s="61"/>
-      <c r="M1" s="61"/>
-      <c r="N1" s="61"/>
-      <c r="O1" s="61"/>
+      <c r="K1" s="51"/>
+      <c r="L1" s="51"/>
+      <c r="M1" s="51"/>
+      <c r="N1" s="51"/>
+      <c r="O1" s="51"/>
       <c r="P1"/>
       <c r="Q1"/>
       <c r="R1"/>
@@ -2566,7 +2582,7 @@
       <c r="AVE1"/>
       <c r="AVF1"/>
     </row>
-    <row r="2" spans="1:1254" s="3" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1254" s="3" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="62" t="s">
         <v>8</v>
       </c>
@@ -3828,35 +3844,35 @@
       <c r="A3" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="17">
+      <c r="B3" s="16">
         <v>54.37</v>
       </c>
-      <c r="C3" s="20">
+      <c r="C3" s="19">
         <v>1</v>
       </c>
-      <c r="D3" s="17">
+      <c r="D3" s="16">
         <f>B3*C3</f>
         <v>54.37</v>
       </c>
-      <c r="E3" s="21" t="s">
+      <c r="E3" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="F3" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="20" t="s">
+      <c r="G3" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="22"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="57" t="s">
+      <c r="H3" s="54"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="K3" s="57"/>
-      <c r="L3" s="57"/>
-      <c r="M3" s="57"/>
-      <c r="N3" s="57"/>
-      <c r="O3" s="57"/>
+      <c r="K3" s="48"/>
+      <c r="L3" s="48"/>
+      <c r="M3" s="48"/>
+      <c r="N3" s="48"/>
+      <c r="O3" s="48"/>
       <c r="FS3"/>
       <c r="FT3"/>
       <c r="FU3"/>
@@ -4712,35 +4728,35 @@
       <c r="A4" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="17">
+      <c r="B4" s="16">
         <v>54.93</v>
       </c>
-      <c r="C4" s="20">
+      <c r="C4" s="19">
         <v>1</v>
       </c>
-      <c r="D4" s="17">
+      <c r="D4" s="16">
         <f t="shared" ref="D4:D5" si="0">B4*C4</f>
         <v>54.93</v>
       </c>
-      <c r="E4" s="21" t="s">
+      <c r="E4" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="21" t="s">
+      <c r="F4" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="20" t="s">
+      <c r="G4" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="22"/>
-      <c r="I4" s="23"/>
-      <c r="J4" s="57" t="s">
+      <c r="H4" s="54"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="K4" s="57"/>
-      <c r="L4" s="57"/>
-      <c r="M4" s="57"/>
-      <c r="N4" s="57"/>
-      <c r="O4" s="57"/>
+      <c r="K4" s="48"/>
+      <c r="L4" s="48"/>
+      <c r="M4" s="48"/>
+      <c r="N4" s="48"/>
+      <c r="O4" s="48"/>
       <c r="FS4"/>
       <c r="FT4"/>
       <c r="FU4"/>
@@ -5596,35 +5612,35 @@
       <c r="A5" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="19">
+      <c r="B5" s="18">
         <v>53.87</v>
       </c>
-      <c r="C5" s="20">
+      <c r="C5" s="19">
         <v>1</v>
       </c>
-      <c r="D5" s="17">
+      <c r="D5" s="16">
         <f t="shared" si="0"/>
         <v>53.87</v>
       </c>
-      <c r="E5" s="21" t="s">
+      <c r="E5" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="21" t="s">
+      <c r="F5" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="20" t="s">
+      <c r="G5" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="22"/>
-      <c r="I5" s="23"/>
-      <c r="J5" s="57" t="s">
+      <c r="H5" s="54"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="K5" s="57"/>
-      <c r="L5" s="57"/>
-      <c r="M5" s="57"/>
-      <c r="N5" s="57"/>
-      <c r="O5" s="57"/>
+      <c r="K5" s="48"/>
+      <c r="L5" s="48"/>
+      <c r="M5" s="48"/>
+      <c r="N5" s="48"/>
+      <c r="O5" s="48"/>
       <c r="FS5"/>
       <c r="FT5"/>
       <c r="FU5"/>
@@ -6476,24 +6492,24 @@
       <c r="AMI5"/>
       <c r="AMJ5"/>
     </row>
-    <row r="6" spans="1:1254" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="60" t="s">
-        <v>18</v>
+    <row r="6" spans="1:1254" s="4" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="62" t="s">
+        <v>154</v>
       </c>
-      <c r="B6" s="60"/>
-      <c r="C6" s="60"/>
-      <c r="D6" s="60"/>
-      <c r="E6" s="60"/>
-      <c r="F6" s="60"/>
-      <c r="G6" s="60"/>
-      <c r="H6" s="60"/>
-      <c r="I6" s="60"/>
-      <c r="J6" s="60"/>
-      <c r="K6" s="60"/>
-      <c r="L6" s="60"/>
-      <c r="M6" s="60"/>
-      <c r="N6" s="60"/>
-      <c r="O6" s="60"/>
+      <c r="B6" s="62"/>
+      <c r="C6" s="62"/>
+      <c r="D6" s="62"/>
+      <c r="E6" s="62"/>
+      <c r="F6" s="62"/>
+      <c r="G6" s="62"/>
+      <c r="H6" s="62"/>
+      <c r="I6" s="62"/>
+      <c r="J6" s="62"/>
+      <c r="K6" s="62"/>
+      <c r="L6" s="62"/>
+      <c r="M6" s="62"/>
+      <c r="N6" s="62"/>
+      <c r="O6" s="62"/>
       <c r="P6"/>
       <c r="Q6"/>
       <c r="R6"/>
@@ -7735,40 +7751,40 @@
       <c r="AVF6"/>
     </row>
     <row r="7" spans="1:1254" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="24" t="s">
-        <v>19</v>
+      <c r="A7" s="22" t="s">
+        <v>18</v>
       </c>
-      <c r="B7" s="17">
+      <c r="B7" s="16">
         <v>6.72</v>
       </c>
-      <c r="C7" s="20">
+      <c r="C7" s="19">
         <v>1</v>
       </c>
-      <c r="D7" s="17">
+      <c r="D7" s="16">
         <f t="shared" ref="D7:D21" si="1">B7*C7</f>
         <v>6.72</v>
       </c>
-      <c r="E7" s="21" t="s">
+      <c r="E7" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="25" t="s">
+      <c r="G7" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="55" t="s">
+        <v>142</v>
+      </c>
+      <c r="I7" s="24"/>
+      <c r="J7" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="G7" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="H7" s="26" t="s">
-        <v>144</v>
-      </c>
-      <c r="I7" s="27"/>
-      <c r="J7" s="57" t="s">
-        <v>22</v>
-      </c>
-      <c r="K7" s="57"/>
-      <c r="L7" s="57"/>
-      <c r="M7" s="57"/>
-      <c r="N7" s="57"/>
-      <c r="O7" s="57"/>
+      <c r="K7" s="48"/>
+      <c r="L7" s="48"/>
+      <c r="M7" s="48"/>
+      <c r="N7" s="48"/>
+      <c r="O7" s="48"/>
       <c r="FS7"/>
       <c r="FT7"/>
       <c r="FU7"/>
@@ -8621,36 +8637,36 @@
       <c r="AMJ7"/>
     </row>
     <row r="8" spans="1:1254" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="28" t="s">
-        <v>23</v>
+      <c r="A8" s="25" t="s">
+        <v>22</v>
       </c>
-      <c r="B8" s="18">
+      <c r="B8" s="17">
         <v>29.94</v>
       </c>
-      <c r="C8" s="29">
+      <c r="C8" s="26">
         <v>1</v>
       </c>
-      <c r="D8" s="17">
+      <c r="D8" s="16">
         <f t="shared" si="1"/>
         <v>29.94</v>
       </c>
-      <c r="E8" s="21" t="s">
-        <v>20</v>
+      <c r="E8" s="20" t="s">
+        <v>19</v>
       </c>
-      <c r="F8" s="25" t="s">
-        <v>24</v>
+      <c r="F8" s="23" t="s">
+        <v>23</v>
       </c>
-      <c r="G8" s="20" t="s">
+      <c r="G8" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H8" s="30"/>
-      <c r="I8" s="27"/>
-      <c r="J8" s="57"/>
-      <c r="K8" s="57"/>
-      <c r="L8" s="57"/>
-      <c r="M8" s="57"/>
-      <c r="N8" s="57"/>
-      <c r="O8" s="57"/>
+      <c r="H8" s="56"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="48"/>
+      <c r="K8" s="48"/>
+      <c r="L8" s="48"/>
+      <c r="M8" s="48"/>
+      <c r="N8" s="48"/>
+      <c r="O8" s="48"/>
       <c r="FS8"/>
       <c r="FT8"/>
       <c r="FU8"/>
@@ -9503,36 +9519,36 @@
       <c r="AMJ8"/>
     </row>
     <row r="9" spans="1:1254" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="28" t="s">
-        <v>25</v>
+      <c r="A9" s="25" t="s">
+        <v>24</v>
       </c>
-      <c r="B9" s="17">
+      <c r="B9" s="16">
         <v>6.87</v>
       </c>
-      <c r="C9" s="20">
+      <c r="C9" s="19">
         <v>2</v>
       </c>
-      <c r="D9" s="17">
+      <c r="D9" s="16">
         <f t="shared" si="1"/>
         <v>13.74</v>
       </c>
-      <c r="E9" s="21" t="s">
-        <v>20</v>
+      <c r="E9" s="20" t="s">
+        <v>19</v>
       </c>
-      <c r="F9" s="25" t="s">
-        <v>26</v>
+      <c r="F9" s="23" t="s">
+        <v>25</v>
       </c>
-      <c r="G9" s="20" t="s">
+      <c r="G9" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H9" s="30"/>
-      <c r="I9" s="27"/>
-      <c r="J9" s="57"/>
-      <c r="K9" s="57"/>
-      <c r="L9" s="57"/>
-      <c r="M9" s="57"/>
-      <c r="N9" s="57"/>
-      <c r="O9" s="57"/>
+      <c r="H9" s="56"/>
+      <c r="I9" s="24"/>
+      <c r="J9" s="48"/>
+      <c r="K9" s="48"/>
+      <c r="L9" s="48"/>
+      <c r="M9" s="48"/>
+      <c r="N9" s="48"/>
+      <c r="O9" s="48"/>
       <c r="FS9"/>
       <c r="FT9"/>
       <c r="FU9"/>
@@ -10385,38 +10401,38 @@
       <c r="AMJ9"/>
     </row>
     <row r="10" spans="1:1254" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="28" t="s">
-        <v>27</v>
+      <c r="A10" s="25" t="s">
+        <v>26</v>
       </c>
-      <c r="B10" s="17">
+      <c r="B10" s="16">
         <v>17.12</v>
       </c>
-      <c r="C10" s="20">
+      <c r="C10" s="19">
         <v>2</v>
       </c>
-      <c r="D10" s="17">
+      <c r="D10" s="16">
         <f t="shared" si="1"/>
         <v>34.24</v>
       </c>
-      <c r="E10" s="21" t="s">
-        <v>20</v>
+      <c r="E10" s="20" t="s">
+        <v>19</v>
       </c>
-      <c r="F10" s="25" t="s">
-        <v>28</v>
+      <c r="F10" s="23" t="s">
+        <v>27</v>
       </c>
-      <c r="G10" s="20" t="s">
+      <c r="G10" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H10" s="26" t="s">
-        <v>144</v>
+      <c r="H10" s="55" t="s">
+        <v>142</v>
       </c>
-      <c r="I10" s="27"/>
-      <c r="J10" s="57"/>
-      <c r="K10" s="57"/>
-      <c r="L10" s="57"/>
-      <c r="M10" s="57"/>
-      <c r="N10" s="57"/>
-      <c r="O10" s="57"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="48"/>
+      <c r="K10" s="48"/>
+      <c r="L10" s="48"/>
+      <c r="M10" s="48"/>
+      <c r="N10" s="48"/>
+      <c r="O10" s="48"/>
       <c r="FS10"/>
       <c r="FT10"/>
       <c r="FU10"/>
@@ -11269,40 +11285,40 @@
       <c r="AMJ10"/>
     </row>
     <row r="11" spans="1:1254" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="28" t="s">
-        <v>29</v>
+      <c r="A11" s="25" t="s">
+        <v>28</v>
       </c>
-      <c r="B11" s="17">
+      <c r="B11" s="16">
         <v>4.04</v>
       </c>
-      <c r="C11" s="20">
+      <c r="C11" s="19">
         <v>2</v>
       </c>
-      <c r="D11" s="17">
+      <c r="D11" s="16">
         <f t="shared" si="1"/>
         <v>8.08</v>
       </c>
-      <c r="E11" s="21" t="s">
-        <v>20</v>
+      <c r="E11" s="20" t="s">
+        <v>19</v>
       </c>
-      <c r="F11" s="25" t="s">
+      <c r="F11" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="G11" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="H11" s="55" t="s">
+        <v>142</v>
+      </c>
+      <c r="I11" s="24"/>
+      <c r="J11" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="G11" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="H11" s="26" t="s">
-        <v>144</v>
-      </c>
-      <c r="I11" s="27"/>
-      <c r="J11" s="57" t="s">
-        <v>31</v>
-      </c>
-      <c r="K11" s="57"/>
-      <c r="L11" s="57"/>
-      <c r="M11" s="57"/>
-      <c r="N11" s="57"/>
-      <c r="O11" s="57"/>
+      <c r="K11" s="48"/>
+      <c r="L11" s="48"/>
+      <c r="M11" s="48"/>
+      <c r="N11" s="48"/>
+      <c r="O11" s="48"/>
       <c r="FS11"/>
       <c r="FT11"/>
       <c r="FU11"/>
@@ -12155,38 +12171,38 @@
       <c r="AMJ11"/>
     </row>
     <row r="12" spans="1:1254" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="28" t="s">
-        <v>153</v>
+      <c r="A12" s="25" t="s">
+        <v>151</v>
       </c>
-      <c r="B12" s="17">
+      <c r="B12" s="16">
         <v>8.11</v>
       </c>
-      <c r="C12" s="20">
+      <c r="C12" s="19">
         <v>2</v>
       </c>
-      <c r="D12" s="17">
+      <c r="D12" s="16">
         <f t="shared" si="1"/>
         <v>16.22</v>
       </c>
-      <c r="E12" s="21" t="s">
-        <v>20</v>
+      <c r="E12" s="20" t="s">
+        <v>19</v>
       </c>
-      <c r="F12" s="25" t="s">
-        <v>32</v>
+      <c r="F12" s="23" t="s">
+        <v>31</v>
       </c>
-      <c r="G12" s="20" t="s">
+      <c r="G12" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H12" s="30"/>
-      <c r="I12" s="27"/>
-      <c r="J12" s="57" t="s">
-        <v>152</v>
+      <c r="H12" s="56"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="48" t="s">
+        <v>150</v>
       </c>
-      <c r="K12" s="57"/>
-      <c r="L12" s="57"/>
-      <c r="M12" s="57"/>
-      <c r="N12" s="57"/>
-      <c r="O12" s="57"/>
+      <c r="K12" s="48"/>
+      <c r="L12" s="48"/>
+      <c r="M12" s="48"/>
+      <c r="N12" s="48"/>
+      <c r="O12" s="48"/>
       <c r="FS12"/>
       <c r="FT12"/>
       <c r="FU12"/>
@@ -13039,38 +13055,38 @@
       <c r="AMJ12"/>
     </row>
     <row r="13" spans="1:1254" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="28" t="s">
-        <v>33</v>
+      <c r="A13" s="25" t="s">
+        <v>32</v>
       </c>
-      <c r="B13" s="17">
+      <c r="B13" s="16">
         <v>3.68</v>
       </c>
-      <c r="C13" s="20">
+      <c r="C13" s="19">
         <v>1</v>
       </c>
-      <c r="D13" s="17">
+      <c r="D13" s="16">
         <f t="shared" si="1"/>
         <v>3.68</v>
       </c>
-      <c r="E13" s="21" t="s">
-        <v>20</v>
+      <c r="E13" s="20" t="s">
+        <v>19</v>
       </c>
-      <c r="F13" s="25" t="s">
+      <c r="F13" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="G13" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="H13" s="56"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="G13" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="H13" s="30"/>
-      <c r="I13" s="27"/>
-      <c r="J13" s="57" t="s">
-        <v>35</v>
-      </c>
-      <c r="K13" s="57"/>
-      <c r="L13" s="57"/>
-      <c r="M13" s="57"/>
-      <c r="N13" s="57"/>
-      <c r="O13" s="57"/>
+      <c r="K13" s="48"/>
+      <c r="L13" s="48"/>
+      <c r="M13" s="48"/>
+      <c r="N13" s="48"/>
+      <c r="O13" s="48"/>
       <c r="FS13"/>
       <c r="FT13"/>
       <c r="FU13"/>
@@ -13923,38 +13939,38 @@
       <c r="AMJ13"/>
     </row>
     <row r="14" spans="1:1254" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="28" t="s">
-        <v>154</v>
+      <c r="A14" s="25" t="s">
+        <v>152</v>
       </c>
-      <c r="B14" s="17">
+      <c r="B14" s="16">
         <v>6.01</v>
       </c>
-      <c r="C14" s="20">
+      <c r="C14" s="19">
         <v>1</v>
       </c>
-      <c r="D14" s="17">
+      <c r="D14" s="16">
         <f t="shared" si="1"/>
         <v>6.01</v>
       </c>
-      <c r="E14" s="21" t="s">
-        <v>20</v>
+      <c r="E14" s="20" t="s">
+        <v>19</v>
       </c>
-      <c r="F14" s="25" t="s">
-        <v>36</v>
+      <c r="F14" s="23" t="s">
+        <v>35</v>
       </c>
-      <c r="G14" s="20" t="s">
+      <c r="G14" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H14" s="30"/>
-      <c r="I14" s="27"/>
-      <c r="J14" s="57" t="s">
-        <v>155</v>
+      <c r="H14" s="56"/>
+      <c r="I14" s="24"/>
+      <c r="J14" s="48" t="s">
+        <v>153</v>
       </c>
-      <c r="K14" s="57"/>
-      <c r="L14" s="57"/>
-      <c r="M14" s="57"/>
-      <c r="N14" s="57"/>
-      <c r="O14" s="57"/>
+      <c r="K14" s="48"/>
+      <c r="L14" s="48"/>
+      <c r="M14" s="48"/>
+      <c r="N14" s="48"/>
+      <c r="O14" s="48"/>
       <c r="FS14"/>
       <c r="FT14"/>
       <c r="FU14"/>
@@ -14807,38 +14823,38 @@
       <c r="AMJ14"/>
     </row>
     <row r="15" spans="1:1254" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="28" t="s">
-        <v>37</v>
+      <c r="A15" s="25" t="s">
+        <v>36</v>
       </c>
-      <c r="B15" s="17">
+      <c r="B15" s="16">
         <v>9.77</v>
       </c>
-      <c r="C15" s="20">
+      <c r="C15" s="19">
         <v>1</v>
       </c>
-      <c r="D15" s="17">
+      <c r="D15" s="16">
         <f t="shared" si="1"/>
         <v>9.77</v>
       </c>
-      <c r="E15" s="21" t="s">
-        <v>20</v>
+      <c r="E15" s="20" t="s">
+        <v>19</v>
       </c>
-      <c r="F15" s="25" t="s">
+      <c r="F15" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="G15" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="H15" s="56"/>
+      <c r="I15" s="24"/>
+      <c r="J15" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="G15" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="H15" s="30"/>
-      <c r="I15" s="27"/>
-      <c r="J15" s="57" t="s">
-        <v>39</v>
-      </c>
-      <c r="K15" s="57"/>
-      <c r="L15" s="57"/>
-      <c r="M15" s="57"/>
-      <c r="N15" s="57"/>
-      <c r="O15" s="57"/>
+      <c r="K15" s="48"/>
+      <c r="L15" s="48"/>
+      <c r="M15" s="48"/>
+      <c r="N15" s="48"/>
+      <c r="O15" s="48"/>
       <c r="FS15"/>
       <c r="FT15"/>
       <c r="FU15"/>
@@ -15691,36 +15707,36 @@
       <c r="AMJ15"/>
     </row>
     <row r="16" spans="1:1254" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="28" t="s">
-        <v>40</v>
+      <c r="A16" s="25" t="s">
+        <v>39</v>
       </c>
-      <c r="B16" s="17">
+      <c r="B16" s="16">
         <v>5.7</v>
       </c>
-      <c r="C16" s="20">
+      <c r="C16" s="19">
         <v>3</v>
       </c>
-      <c r="D16" s="17">
+      <c r="D16" s="16">
         <f t="shared" si="1"/>
         <v>17.100000000000001</v>
       </c>
-      <c r="E16" s="21" t="s">
-        <v>20</v>
+      <c r="E16" s="20" t="s">
+        <v>19</v>
       </c>
-      <c r="F16" s="25" t="s">
-        <v>41</v>
+      <c r="F16" s="23" t="s">
+        <v>40</v>
       </c>
-      <c r="G16" s="20" t="s">
+      <c r="G16" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H16" s="30"/>
-      <c r="I16" s="27"/>
-      <c r="J16" s="57"/>
-      <c r="K16" s="57"/>
-      <c r="L16" s="57"/>
-      <c r="M16" s="57"/>
-      <c r="N16" s="57"/>
-      <c r="O16" s="57"/>
+      <c r="H16" s="56"/>
+      <c r="I16" s="24"/>
+      <c r="J16" s="48"/>
+      <c r="K16" s="48"/>
+      <c r="L16" s="48"/>
+      <c r="M16" s="48"/>
+      <c r="N16" s="48"/>
+      <c r="O16" s="48"/>
       <c r="FS16"/>
       <c r="FT16"/>
       <c r="FU16"/>
@@ -16573,38 +16589,38 @@
       <c r="AMJ16"/>
     </row>
     <row r="17" spans="1:1254" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="28" t="s">
-        <v>151</v>
+      <c r="A17" s="25" t="s">
+        <v>149</v>
       </c>
-      <c r="B17" s="17">
+      <c r="B17" s="16">
         <v>20.7</v>
       </c>
-      <c r="C17" s="20">
+      <c r="C17" s="19">
         <v>2</v>
       </c>
-      <c r="D17" s="17">
+      <c r="D17" s="16">
         <f t="shared" si="1"/>
         <v>41.4</v>
       </c>
-      <c r="E17" s="21" t="s">
-        <v>20</v>
+      <c r="E17" s="20" t="s">
+        <v>19</v>
       </c>
-      <c r="F17" s="25" t="s">
-        <v>42</v>
+      <c r="F17" s="23" t="s">
+        <v>41</v>
       </c>
-      <c r="G17" s="20" t="s">
+      <c r="G17" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H17" s="30"/>
-      <c r="I17" s="27"/>
-      <c r="J17" s="57" t="s">
-        <v>147</v>
+      <c r="H17" s="56"/>
+      <c r="I17" s="24"/>
+      <c r="J17" s="48" t="s">
+        <v>145</v>
       </c>
-      <c r="K17" s="57"/>
-      <c r="L17" s="57"/>
-      <c r="M17" s="57"/>
-      <c r="N17" s="57"/>
-      <c r="O17" s="57"/>
+      <c r="K17" s="48"/>
+      <c r="L17" s="48"/>
+      <c r="M17" s="48"/>
+      <c r="N17" s="48"/>
+      <c r="O17" s="48"/>
       <c r="FS17"/>
       <c r="FT17"/>
       <c r="FU17"/>
@@ -17457,36 +17473,36 @@
       <c r="AMJ17"/>
     </row>
     <row r="18" spans="1:1254" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="28" t="s">
-        <v>148</v>
+      <c r="A18" s="25" t="s">
+        <v>146</v>
       </c>
-      <c r="B18" s="17">
+      <c r="B18" s="16">
         <v>5.68</v>
       </c>
-      <c r="C18" s="20">
+      <c r="C18" s="19">
         <v>2</v>
       </c>
-      <c r="D18" s="17">
+      <c r="D18" s="16">
         <f t="shared" si="1"/>
         <v>11.36</v>
       </c>
-      <c r="E18" s="21" t="s">
-        <v>20</v>
+      <c r="E18" s="20" t="s">
+        <v>19</v>
       </c>
-      <c r="F18" s="25" t="s">
-        <v>43</v>
+      <c r="F18" s="23" t="s">
+        <v>42</v>
       </c>
-      <c r="G18" s="20" t="s">
+      <c r="G18" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H18" s="30"/>
-      <c r="I18" s="27"/>
-      <c r="J18" s="57"/>
-      <c r="K18" s="57"/>
-      <c r="L18" s="57"/>
-      <c r="M18" s="57"/>
-      <c r="N18" s="57"/>
-      <c r="O18" s="57"/>
+      <c r="H18" s="56"/>
+      <c r="I18" s="24"/>
+      <c r="J18" s="48"/>
+      <c r="K18" s="48"/>
+      <c r="L18" s="48"/>
+      <c r="M18" s="48"/>
+      <c r="N18" s="48"/>
+      <c r="O18" s="48"/>
       <c r="FS18"/>
       <c r="FT18"/>
       <c r="FU18"/>
@@ -18339,40 +18355,40 @@
       <c r="AMJ18"/>
     </row>
     <row r="19" spans="1:1254" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="28" t="s">
-        <v>149</v>
+      <c r="A19" s="25" t="s">
+        <v>147</v>
       </c>
-      <c r="B19" s="17">
+      <c r="B19" s="16">
         <v>2.6</v>
       </c>
-      <c r="C19" s="29">
+      <c r="C19" s="26">
         <v>3</v>
       </c>
-      <c r="D19" s="17">
+      <c r="D19" s="16">
         <f t="shared" si="1"/>
         <v>7.8000000000000007</v>
       </c>
-      <c r="E19" s="21" t="s">
-        <v>20</v>
+      <c r="E19" s="20" t="s">
+        <v>19</v>
       </c>
-      <c r="F19" s="25" t="s">
-        <v>44</v>
+      <c r="F19" s="23" t="s">
+        <v>43</v>
       </c>
-      <c r="G19" s="20" t="s">
+      <c r="G19" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H19" s="26" t="s">
-        <v>144</v>
+      <c r="H19" s="55" t="s">
+        <v>142</v>
       </c>
-      <c r="I19" s="27"/>
-      <c r="J19" s="57" t="s">
-        <v>150</v>
+      <c r="I19" s="24"/>
+      <c r="J19" s="48" t="s">
+        <v>148</v>
       </c>
-      <c r="K19" s="57"/>
-      <c r="L19" s="57"/>
-      <c r="M19" s="57"/>
-      <c r="N19" s="57"/>
-      <c r="O19" s="57"/>
+      <c r="K19" s="48"/>
+      <c r="L19" s="48"/>
+      <c r="M19" s="48"/>
+      <c r="N19" s="48"/>
+      <c r="O19" s="48"/>
       <c r="FS19"/>
       <c r="FT19"/>
       <c r="FU19"/>
@@ -19225,40 +19241,40 @@
       <c r="AMJ19"/>
     </row>
     <row r="20" spans="1:1254" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="31" t="s">
-        <v>123</v>
+      <c r="A20" s="27" t="s">
+        <v>121</v>
       </c>
-      <c r="B20" s="15">
+      <c r="B20" s="14">
         <v>23.82</v>
       </c>
-      <c r="C20" s="32">
+      <c r="C20" s="28">
         <v>1</v>
       </c>
-      <c r="D20" s="17">
+      <c r="D20" s="16">
         <f t="shared" si="1"/>
         <v>23.82</v>
       </c>
-      <c r="E20" s="33" t="s">
-        <v>20</v>
+      <c r="E20" s="29" t="s">
+        <v>19</v>
       </c>
-      <c r="F20" s="34" t="s">
-        <v>124</v>
+      <c r="F20" s="30" t="s">
+        <v>122</v>
       </c>
-      <c r="G20" s="32" t="s">
-        <v>86</v>
+      <c r="G20" s="28" t="s">
+        <v>84</v>
       </c>
-      <c r="H20" s="26" t="s">
-        <v>144</v>
+      <c r="H20" s="55" t="s">
+        <v>142</v>
       </c>
-      <c r="I20" s="35"/>
-      <c r="J20" s="57" t="s">
-        <v>125</v>
+      <c r="I20" s="31"/>
+      <c r="J20" s="48" t="s">
+        <v>123</v>
       </c>
-      <c r="K20" s="57"/>
-      <c r="L20" s="57"/>
-      <c r="M20" s="57"/>
-      <c r="N20" s="57"/>
-      <c r="O20" s="57"/>
+      <c r="K20" s="48"/>
+      <c r="L20" s="48"/>
+      <c r="M20" s="48"/>
+      <c r="N20" s="48"/>
+      <c r="O20" s="48"/>
       <c r="FS20"/>
       <c r="FT20"/>
       <c r="FU20"/>
@@ -20111,40 +20127,40 @@
       <c r="AMJ20"/>
     </row>
     <row r="21" spans="1:1254" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="28" t="s">
-        <v>74</v>
+      <c r="A21" s="25" t="s">
+        <v>73</v>
       </c>
-      <c r="B21" s="17">
+      <c r="B21" s="16">
         <v>25.93</v>
       </c>
-      <c r="C21" s="29">
+      <c r="C21" s="26">
         <v>1</v>
       </c>
-      <c r="D21" s="17">
+      <c r="D21" s="16">
         <f t="shared" si="1"/>
         <v>25.93</v>
       </c>
-      <c r="E21" s="21" t="s">
-        <v>20</v>
+      <c r="E21" s="20" t="s">
+        <v>19</v>
       </c>
-      <c r="F21" s="25" t="s">
-        <v>75</v>
+      <c r="F21" s="23" t="s">
+        <v>74</v>
       </c>
-      <c r="G21" s="20" t="s">
+      <c r="G21" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H21" s="26" t="s">
-        <v>144</v>
+      <c r="H21" s="55" t="s">
+        <v>142</v>
       </c>
-      <c r="I21" s="36"/>
-      <c r="J21" s="57" t="s">
-        <v>76</v>
+      <c r="I21" s="32"/>
+      <c r="J21" s="48" t="s">
+        <v>155</v>
       </c>
-      <c r="K21" s="57"/>
-      <c r="L21" s="57"/>
-      <c r="M21" s="57"/>
-      <c r="N21" s="57"/>
-      <c r="O21" s="57"/>
+      <c r="K21" s="48"/>
+      <c r="L21" s="48"/>
+      <c r="M21" s="48"/>
+      <c r="N21" s="48"/>
+      <c r="O21" s="48"/>
       <c r="FS21"/>
       <c r="FT21"/>
       <c r="FU21"/>
@@ -20996,24 +21012,24 @@
       <c r="AMI21"/>
       <c r="AMJ21"/>
     </row>
-    <row r="22" spans="1:1254" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="60" t="s">
-        <v>45</v>
+    <row r="22" spans="1:1254" s="4" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="62" t="s">
+        <v>44</v>
       </c>
-      <c r="B22" s="60"/>
-      <c r="C22" s="60"/>
-      <c r="D22" s="60"/>
-      <c r="E22" s="60"/>
-      <c r="F22" s="60"/>
-      <c r="G22" s="60"/>
-      <c r="H22" s="60"/>
-      <c r="I22" s="60"/>
-      <c r="J22" s="60"/>
-      <c r="K22" s="60"/>
-      <c r="L22" s="60"/>
-      <c r="M22" s="60"/>
-      <c r="N22" s="60"/>
-      <c r="O22" s="60"/>
+      <c r="B22" s="62"/>
+      <c r="C22" s="62"/>
+      <c r="D22" s="62"/>
+      <c r="E22" s="62"/>
+      <c r="F22" s="62"/>
+      <c r="G22" s="62"/>
+      <c r="H22" s="62"/>
+      <c r="I22" s="62"/>
+      <c r="J22" s="62"/>
+      <c r="K22" s="62"/>
+      <c r="L22" s="62"/>
+      <c r="M22" s="62"/>
+      <c r="N22" s="62"/>
+      <c r="O22" s="62"/>
       <c r="P22"/>
       <c r="Q22"/>
       <c r="R22"/>
@@ -22256,37 +22272,37 @@
     </row>
     <row r="23" spans="1:1254" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
-      <c r="B23" s="17">
+      <c r="B23" s="16">
         <v>97.89</v>
       </c>
-      <c r="C23" s="20">
+      <c r="C23" s="19">
         <v>1</v>
       </c>
-      <c r="D23" s="17">
+      <c r="D23" s="16">
         <f>B23*C23</f>
         <v>97.89</v>
       </c>
-      <c r="E23" s="21" t="s">
-        <v>47</v>
+      <c r="E23" s="20" t="s">
+        <v>46</v>
       </c>
-      <c r="F23" s="21">
+      <c r="F23" s="20">
         <v>9052000029</v>
       </c>
-      <c r="G23" s="20" t="s">
+      <c r="G23" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H23" s="26" t="s">
-        <v>144</v>
+      <c r="H23" s="55" t="s">
+        <v>142</v>
       </c>
-      <c r="I23" s="37"/>
-      <c r="J23" s="57"/>
-      <c r="K23" s="57"/>
-      <c r="L23" s="57"/>
-      <c r="M23" s="57"/>
-      <c r="N23" s="57"/>
-      <c r="O23" s="57"/>
+      <c r="I23" s="33"/>
+      <c r="J23" s="48"/>
+      <c r="K23" s="48"/>
+      <c r="L23" s="48"/>
+      <c r="M23" s="48"/>
+      <c r="N23" s="48"/>
+      <c r="O23" s="48"/>
       <c r="FS23"/>
       <c r="FT23"/>
       <c r="FU23"/>
@@ -23140,37 +23156,37 @@
     </row>
     <row r="24" spans="1:1254" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
-      <c r="B24" s="17">
+      <c r="B24" s="16">
         <v>247.07</v>
       </c>
-      <c r="C24" s="20">
+      <c r="C24" s="19">
         <v>1</v>
       </c>
-      <c r="D24" s="17">
+      <c r="D24" s="16">
         <f t="shared" ref="D24:D28" si="2">B24*C24</f>
         <v>247.07</v>
       </c>
-      <c r="E24" s="21" t="s">
+      <c r="E24" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="F24" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="F24" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="G24" s="20" t="s">
+      <c r="G24" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H24" s="26" t="s">
-        <v>144</v>
+      <c r="H24" s="55" t="s">
+        <v>142</v>
       </c>
-      <c r="I24" s="37"/>
-      <c r="J24" s="57"/>
-      <c r="K24" s="57"/>
-      <c r="L24" s="57"/>
-      <c r="M24" s="57"/>
-      <c r="N24" s="57"/>
-      <c r="O24" s="57"/>
+      <c r="I24" s="33"/>
+      <c r="J24" s="48"/>
+      <c r="K24" s="48"/>
+      <c r="L24" s="48"/>
+      <c r="M24" s="48"/>
+      <c r="N24" s="48"/>
+      <c r="O24" s="48"/>
       <c r="FS24"/>
       <c r="FT24"/>
       <c r="FU24"/>
@@ -24024,37 +24040,37 @@
     </row>
     <row r="25" spans="1:1254" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
-      <c r="B25" s="17">
+      <c r="B25" s="16">
         <v>3.5</v>
       </c>
-      <c r="C25" s="20">
+      <c r="C25" s="19">
         <v>2</v>
       </c>
-      <c r="D25" s="17">
+      <c r="D25" s="16">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="E25" s="21" t="s">
-        <v>47</v>
+      <c r="E25" s="20" t="s">
+        <v>46</v>
       </c>
-      <c r="F25" s="21" t="s">
-        <v>50</v>
+      <c r="F25" s="20" t="s">
+        <v>49</v>
       </c>
-      <c r="G25" s="20" t="s">
+      <c r="G25" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H25" s="26" t="s">
-        <v>144</v>
+      <c r="H25" s="55" t="s">
+        <v>142</v>
       </c>
-      <c r="I25" s="37"/>
-      <c r="J25" s="57"/>
-      <c r="K25" s="57"/>
-      <c r="L25" s="57"/>
-      <c r="M25" s="57"/>
-      <c r="N25" s="57"/>
-      <c r="O25" s="57"/>
+      <c r="I25" s="33"/>
+      <c r="J25" s="48"/>
+      <c r="K25" s="48"/>
+      <c r="L25" s="48"/>
+      <c r="M25" s="48"/>
+      <c r="N25" s="48"/>
+      <c r="O25" s="48"/>
       <c r="FS25"/>
       <c r="FT25"/>
       <c r="FU25"/>
@@ -24908,37 +24924,37 @@
     </row>
     <row r="26" spans="1:1254" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
-      <c r="B26" s="17">
+      <c r="B26" s="16">
         <v>18</v>
       </c>
-      <c r="C26" s="20">
+      <c r="C26" s="19">
         <v>1</v>
       </c>
-      <c r="D26" s="17">
+      <c r="D26" s="16">
         <f t="shared" si="2"/>
         <v>18</v>
       </c>
-      <c r="E26" s="21" t="s">
-        <v>47</v>
+      <c r="E26" s="20" t="s">
+        <v>46</v>
       </c>
-      <c r="F26" s="21" t="s">
-        <v>52</v>
+      <c r="F26" s="20" t="s">
+        <v>51</v>
       </c>
-      <c r="G26" s="20" t="s">
+      <c r="G26" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H26" s="26" t="s">
-        <v>144</v>
+      <c r="H26" s="55" t="s">
+        <v>142</v>
       </c>
-      <c r="I26" s="37"/>
-      <c r="J26" s="57"/>
-      <c r="K26" s="57"/>
-      <c r="L26" s="57"/>
-      <c r="M26" s="57"/>
-      <c r="N26" s="57"/>
-      <c r="O26" s="57"/>
+      <c r="I26" s="33"/>
+      <c r="J26" s="48"/>
+      <c r="K26" s="48"/>
+      <c r="L26" s="48"/>
+      <c r="M26" s="48"/>
+      <c r="N26" s="48"/>
+      <c r="O26" s="48"/>
       <c r="FS26"/>
       <c r="FT26"/>
       <c r="FU26"/>
@@ -25792,37 +25808,37 @@
     </row>
     <row r="27" spans="1:1254" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
-      <c r="B27" s="17">
+      <c r="B27" s="16">
         <v>157.57</v>
       </c>
-      <c r="C27" s="20">
+      <c r="C27" s="19">
         <v>2</v>
       </c>
-      <c r="D27" s="17">
+      <c r="D27" s="16">
         <f t="shared" si="2"/>
         <v>315.14</v>
       </c>
-      <c r="E27" s="21" t="s">
-        <v>47</v>
+      <c r="E27" s="20" t="s">
+        <v>46</v>
       </c>
-      <c r="F27" s="21" t="s">
-        <v>54</v>
+      <c r="F27" s="20" t="s">
+        <v>53</v>
       </c>
-      <c r="G27" s="20" t="s">
+      <c r="G27" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H27" s="26" t="s">
-        <v>144</v>
+      <c r="H27" s="55" t="s">
+        <v>142</v>
       </c>
-      <c r="I27" s="37"/>
-      <c r="J27" s="57"/>
-      <c r="K27" s="57"/>
-      <c r="L27" s="57"/>
-      <c r="M27" s="57"/>
-      <c r="N27" s="57"/>
-      <c r="O27" s="57"/>
+      <c r="I27" s="33"/>
+      <c r="J27" s="48"/>
+      <c r="K27" s="48"/>
+      <c r="L27" s="48"/>
+      <c r="M27" s="48"/>
+      <c r="N27" s="48"/>
+      <c r="O27" s="48"/>
       <c r="FS27"/>
       <c r="FT27"/>
       <c r="FU27"/>
@@ -26675,38 +26691,38 @@
       <c r="AMJ27"/>
     </row>
     <row r="28" spans="1:1254" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="31" t="s">
-        <v>126</v>
+      <c r="A28" s="27" t="s">
+        <v>124</v>
       </c>
-      <c r="B28" s="15">
+      <c r="B28" s="14">
         <v>153.85</v>
       </c>
-      <c r="C28" s="32">
+      <c r="C28" s="28">
         <v>1</v>
       </c>
-      <c r="D28" s="17">
+      <c r="D28" s="16">
         <f t="shared" si="2"/>
         <v>153.85</v>
       </c>
-      <c r="E28" s="33" t="s">
-        <v>127</v>
+      <c r="E28" s="29" t="s">
+        <v>125</v>
       </c>
-      <c r="F28" s="34" t="s">
-        <v>128</v>
+      <c r="F28" s="30" t="s">
+        <v>126</v>
       </c>
-      <c r="G28" s="32" t="s">
-        <v>86</v>
+      <c r="G28" s="28" t="s">
+        <v>84</v>
       </c>
-      <c r="H28" s="38" t="s">
-        <v>144</v>
+      <c r="H28" s="57" t="s">
+        <v>142</v>
       </c>
-      <c r="I28" s="39"/>
-      <c r="J28" s="57"/>
-      <c r="K28" s="57"/>
-      <c r="L28" s="57"/>
-      <c r="M28" s="57"/>
-      <c r="N28" s="57"/>
-      <c r="O28" s="57"/>
+      <c r="I28" s="34"/>
+      <c r="J28" s="48"/>
+      <c r="K28" s="48"/>
+      <c r="L28" s="48"/>
+      <c r="M28" s="48"/>
+      <c r="N28" s="48"/>
+      <c r="O28" s="48"/>
       <c r="FS28"/>
       <c r="FT28"/>
       <c r="FU28"/>
@@ -27559,23 +27575,23 @@
       <c r="AMJ28"/>
     </row>
     <row r="29" spans="1:1254" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="60" t="s">
-        <v>55</v>
+      <c r="A29" s="49" t="s">
+        <v>54</v>
       </c>
-      <c r="B29" s="60"/>
-      <c r="C29" s="60"/>
-      <c r="D29" s="60"/>
-      <c r="E29" s="60"/>
-      <c r="F29" s="60"/>
-      <c r="G29" s="60"/>
-      <c r="H29" s="60"/>
-      <c r="I29" s="60"/>
-      <c r="J29" s="60"/>
-      <c r="K29" s="60"/>
-      <c r="L29" s="60"/>
-      <c r="M29" s="60"/>
-      <c r="N29" s="60"/>
-      <c r="O29" s="60"/>
+      <c r="B29" s="49"/>
+      <c r="C29" s="49"/>
+      <c r="D29" s="49"/>
+      <c r="E29" s="49"/>
+      <c r="F29" s="49"/>
+      <c r="G29" s="49"/>
+      <c r="H29" s="49"/>
+      <c r="I29" s="49"/>
+      <c r="J29" s="49"/>
+      <c r="K29" s="49"/>
+      <c r="L29" s="49"/>
+      <c r="M29" s="49"/>
+      <c r="N29" s="49"/>
+      <c r="O29" s="49"/>
       <c r="P29"/>
       <c r="Q29"/>
       <c r="R29"/>
@@ -28816,37 +28832,37 @@
       <c r="AVE29"/>
       <c r="AVF29"/>
     </row>
-    <row r="30" spans="1:1254" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:1254" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
-      <c r="B30" s="16">
+      <c r="B30" s="15">
         <v>0</v>
       </c>
-      <c r="C30" s="20">
+      <c r="C30" s="19">
         <v>1</v>
       </c>
-      <c r="D30" s="17">
+      <c r="D30" s="16">
         <f t="shared" ref="D30:D35" si="3">B30*C30</f>
         <v>0</v>
       </c>
-      <c r="E30" s="21" t="s">
+      <c r="E30" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="F30" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="F30" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="G30" s="20" t="s">
+      <c r="G30" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H30" s="22"/>
-      <c r="I30" s="40"/>
-      <c r="J30" s="57"/>
-      <c r="K30" s="57"/>
-      <c r="L30" s="57"/>
-      <c r="M30" s="57"/>
-      <c r="N30" s="57"/>
-      <c r="O30" s="57"/>
+      <c r="H30" s="54"/>
+      <c r="I30" s="35"/>
+      <c r="J30" s="48"/>
+      <c r="K30" s="48"/>
+      <c r="L30" s="48"/>
+      <c r="M30" s="48"/>
+      <c r="N30" s="48"/>
+      <c r="O30" s="48"/>
       <c r="FS30"/>
       <c r="FT30"/>
       <c r="FU30"/>
@@ -29698,37 +29714,37 @@
       <c r="AMI30"/>
       <c r="AMJ30"/>
     </row>
-    <row r="31" spans="1:1254" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:1254" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
-      <c r="B31" s="16">
+      <c r="B31" s="15">
         <v>0</v>
       </c>
-      <c r="C31" s="20">
+      <c r="C31" s="19">
         <v>1</v>
       </c>
-      <c r="D31" s="17">
+      <c r="D31" s="16">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="E31" s="21" t="s">
-        <v>57</v>
+      <c r="E31" s="20" t="s">
+        <v>56</v>
       </c>
-      <c r="F31" s="21" t="s">
-        <v>60</v>
+      <c r="F31" s="20" t="s">
+        <v>59</v>
       </c>
-      <c r="G31" s="20" t="s">
+      <c r="G31" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H31" s="22"/>
-      <c r="I31" s="40"/>
-      <c r="J31" s="57"/>
-      <c r="K31" s="57"/>
-      <c r="L31" s="57"/>
-      <c r="M31" s="57"/>
-      <c r="N31" s="57"/>
-      <c r="O31" s="57"/>
+      <c r="H31" s="54"/>
+      <c r="I31" s="35"/>
+      <c r="J31" s="48"/>
+      <c r="K31" s="48"/>
+      <c r="L31" s="48"/>
+      <c r="M31" s="48"/>
+      <c r="N31" s="48"/>
+      <c r="O31" s="48"/>
       <c r="FS31"/>
       <c r="FT31"/>
       <c r="FU31"/>
@@ -30580,37 +30596,37 @@
       <c r="AMI31"/>
       <c r="AMJ31"/>
     </row>
-    <row r="32" spans="1:1254" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:1254" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
-      <c r="B32" s="16">
+      <c r="B32" s="15">
         <v>0</v>
       </c>
-      <c r="C32" s="20">
+      <c r="C32" s="19">
         <v>1</v>
       </c>
-      <c r="D32" s="17">
+      <c r="D32" s="16">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="E32" s="21" t="s">
-        <v>57</v>
+      <c r="E32" s="20" t="s">
+        <v>56</v>
       </c>
-      <c r="F32" s="21" t="s">
-        <v>62</v>
+      <c r="F32" s="20" t="s">
+        <v>61</v>
       </c>
-      <c r="G32" s="20" t="s">
+      <c r="G32" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H32" s="22"/>
-      <c r="I32" s="40"/>
-      <c r="J32" s="57"/>
-      <c r="K32" s="57"/>
-      <c r="L32" s="57"/>
-      <c r="M32" s="57"/>
-      <c r="N32" s="57"/>
-      <c r="O32" s="57"/>
+      <c r="H32" s="54"/>
+      <c r="I32" s="35"/>
+      <c r="J32" s="48"/>
+      <c r="K32" s="48"/>
+      <c r="L32" s="48"/>
+      <c r="M32" s="48"/>
+      <c r="N32" s="48"/>
+      <c r="O32" s="48"/>
       <c r="FS32"/>
       <c r="FT32"/>
       <c r="FU32"/>
@@ -31462,37 +31478,37 @@
       <c r="AMI32"/>
       <c r="AMJ32"/>
     </row>
-    <row r="33" spans="1:1254" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1254" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
-      <c r="B33" s="16">
+      <c r="B33" s="15">
         <v>0</v>
       </c>
-      <c r="C33" s="20">
+      <c r="C33" s="19">
         <v>1</v>
       </c>
-      <c r="D33" s="17">
+      <c r="D33" s="16">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="E33" s="21" t="s">
-        <v>57</v>
+      <c r="E33" s="20" t="s">
+        <v>56</v>
       </c>
-      <c r="F33" s="21" t="s">
-        <v>64</v>
+      <c r="F33" s="20" t="s">
+        <v>63</v>
       </c>
-      <c r="G33" s="20" t="s">
+      <c r="G33" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H33" s="22"/>
-      <c r="I33" s="40"/>
-      <c r="J33" s="57"/>
-      <c r="K33" s="57"/>
-      <c r="L33" s="57"/>
-      <c r="M33" s="57"/>
-      <c r="N33" s="57"/>
-      <c r="O33" s="57"/>
+      <c r="H33" s="54"/>
+      <c r="I33" s="35"/>
+      <c r="J33" s="48"/>
+      <c r="K33" s="48"/>
+      <c r="L33" s="48"/>
+      <c r="M33" s="48"/>
+      <c r="N33" s="48"/>
+      <c r="O33" s="48"/>
       <c r="FS33"/>
       <c r="FT33"/>
       <c r="FU33"/>
@@ -32344,37 +32360,37 @@
       <c r="AMI33"/>
       <c r="AMJ33"/>
     </row>
-    <row r="34" spans="1:1254" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1254" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
-      <c r="B34" s="16">
+      <c r="B34" s="15">
         <v>0</v>
       </c>
-      <c r="C34" s="20">
+      <c r="C34" s="19">
         <v>1</v>
       </c>
-      <c r="D34" s="17">
+      <c r="D34" s="16">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="E34" s="21" t="s">
-        <v>57</v>
+      <c r="E34" s="20" t="s">
+        <v>56</v>
       </c>
-      <c r="F34" s="21" t="s">
-        <v>66</v>
+      <c r="F34" s="20" t="s">
+        <v>65</v>
       </c>
-      <c r="G34" s="20" t="s">
+      <c r="G34" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H34" s="22"/>
-      <c r="I34" s="40"/>
-      <c r="J34" s="57"/>
-      <c r="K34" s="57"/>
-      <c r="L34" s="57"/>
-      <c r="M34" s="57"/>
-      <c r="N34" s="57"/>
-      <c r="O34" s="57"/>
+      <c r="H34" s="54"/>
+      <c r="I34" s="35"/>
+      <c r="J34" s="48"/>
+      <c r="K34" s="48"/>
+      <c r="L34" s="48"/>
+      <c r="M34" s="48"/>
+      <c r="N34" s="48"/>
+      <c r="O34" s="48"/>
       <c r="FS34"/>
       <c r="FT34"/>
       <c r="FU34"/>
@@ -33226,37 +33242,37 @@
       <c r="AMI34"/>
       <c r="AMJ34"/>
     </row>
-    <row r="35" spans="1:1254" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1254" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
-      <c r="B35" s="16">
+      <c r="B35" s="15">
         <v>0</v>
       </c>
-      <c r="C35" s="20">
+      <c r="C35" s="19">
         <v>1</v>
       </c>
-      <c r="D35" s="17">
+      <c r="D35" s="16">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="E35" s="21" t="s">
-        <v>57</v>
+      <c r="E35" s="20" t="s">
+        <v>56</v>
       </c>
-      <c r="F35" s="21" t="s">
-        <v>68</v>
+      <c r="F35" s="20" t="s">
+        <v>67</v>
       </c>
-      <c r="G35" s="20" t="s">
+      <c r="G35" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H35" s="22"/>
-      <c r="I35" s="40"/>
-      <c r="J35" s="57"/>
-      <c r="K35" s="57"/>
-      <c r="L35" s="57"/>
-      <c r="M35" s="57"/>
-      <c r="N35" s="57"/>
-      <c r="O35" s="57"/>
+      <c r="H35" s="54"/>
+      <c r="I35" s="35"/>
+      <c r="J35" s="48"/>
+      <c r="K35" s="48"/>
+      <c r="L35" s="48"/>
+      <c r="M35" s="48"/>
+      <c r="N35" s="48"/>
+      <c r="O35" s="48"/>
       <c r="FS35"/>
       <c r="FT35"/>
       <c r="FU35"/>
@@ -34108,9 +34124,9 @@
       <c r="AMI35"/>
       <c r="AMJ35"/>
     </row>
-    <row r="36" spans="1:1254" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1254" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="63" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B36" s="63"/>
       <c r="C36" s="63"/>
@@ -34977,38 +34993,38 @@
       <c r="AMI36"/>
       <c r="AMJ36"/>
     </row>
-    <row r="37" spans="1:1254" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:1254" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="10" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
-      <c r="B37" s="16">
+      <c r="B37" s="15">
         <v>3.4495</v>
       </c>
-      <c r="C37" s="20">
+      <c r="C37" s="19">
         <v>2</v>
       </c>
-      <c r="D37" s="17">
+      <c r="D37" s="16">
         <f xml:space="preserve"> C37*O37*B37</f>
         <v>34.494999999999997</v>
       </c>
-      <c r="E37" s="21" t="s">
-        <v>80</v>
+      <c r="E37" s="20" t="s">
+        <v>78</v>
       </c>
-      <c r="F37" s="21" t="s">
-        <v>81</v>
+      <c r="F37" s="20" t="s">
+        <v>79</v>
       </c>
-      <c r="G37" s="20" t="s">
+      <c r="G37" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H37" s="22"/>
-      <c r="I37" s="23"/>
-      <c r="J37" s="56" t="s">
-        <v>136</v>
+      <c r="H37" s="54"/>
+      <c r="I37" s="21"/>
+      <c r="J37" s="53" t="s">
+        <v>134</v>
       </c>
-      <c r="K37" s="56"/>
-      <c r="L37" s="56"/>
-      <c r="M37" s="56"/>
-      <c r="N37" s="56"/>
+      <c r="K37" s="53"/>
+      <c r="L37" s="53"/>
+      <c r="M37" s="53"/>
+      <c r="N37" s="53"/>
       <c r="O37" s="10">
         <v>5</v>
       </c>
@@ -35863,38 +35879,38 @@
       <c r="AMI37"/>
       <c r="AMJ37"/>
     </row>
-    <row r="38" spans="1:1254" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:1254" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="10" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
-      <c r="B38" s="16">
+      <c r="B38" s="15">
         <v>3.45</v>
       </c>
-      <c r="C38" s="20">
+      <c r="C38" s="19">
         <v>2</v>
       </c>
-      <c r="D38" s="17">
+      <c r="D38" s="16">
         <f t="shared" ref="D38:D44" si="4" xml:space="preserve"> C38*O38*B38</f>
         <v>55.2</v>
       </c>
-      <c r="E38" s="21" t="s">
-        <v>80</v>
+      <c r="E38" s="20" t="s">
+        <v>78</v>
       </c>
-      <c r="F38" s="21" t="s">
-        <v>81</v>
+      <c r="F38" s="20" t="s">
+        <v>79</v>
       </c>
-      <c r="G38" s="20" t="s">
+      <c r="G38" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H38" s="22"/>
-      <c r="I38" s="23"/>
-      <c r="J38" s="56" t="s">
-        <v>136</v>
+      <c r="H38" s="54"/>
+      <c r="I38" s="21"/>
+      <c r="J38" s="53" t="s">
+        <v>134</v>
       </c>
-      <c r="K38" s="56"/>
-      <c r="L38" s="56"/>
-      <c r="M38" s="56"/>
-      <c r="N38" s="56"/>
+      <c r="K38" s="53"/>
+      <c r="L38" s="53"/>
+      <c r="M38" s="53"/>
+      <c r="N38" s="53"/>
       <c r="O38" s="10">
         <v>8</v>
       </c>
@@ -36749,38 +36765,38 @@
       <c r="AMI38"/>
       <c r="AMJ38"/>
     </row>
-    <row r="39" spans="1:1254" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:1254" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="10" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
-      <c r="B39" s="16">
+      <c r="B39" s="15">
         <v>3.4504999999999999</v>
       </c>
-      <c r="C39" s="20">
+      <c r="C39" s="19">
         <v>2</v>
       </c>
-      <c r="D39" s="17">
+      <c r="D39" s="16">
         <f t="shared" si="4"/>
         <v>27.603999999999999</v>
       </c>
-      <c r="E39" s="21" t="s">
-        <v>80</v>
+      <c r="E39" s="20" t="s">
+        <v>78</v>
       </c>
-      <c r="F39" s="21" t="s">
-        <v>81</v>
+      <c r="F39" s="20" t="s">
+        <v>79</v>
       </c>
-      <c r="G39" s="20" t="s">
+      <c r="G39" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H39" s="22"/>
-      <c r="I39" s="23"/>
-      <c r="J39" s="56" t="s">
-        <v>136</v>
+      <c r="H39" s="54"/>
+      <c r="I39" s="21"/>
+      <c r="J39" s="53" t="s">
+        <v>134</v>
       </c>
-      <c r="K39" s="56"/>
-      <c r="L39" s="56"/>
-      <c r="M39" s="56"/>
-      <c r="N39" s="56"/>
+      <c r="K39" s="53"/>
+      <c r="L39" s="53"/>
+      <c r="M39" s="53"/>
+      <c r="N39" s="53"/>
       <c r="O39" s="10">
         <v>4</v>
       </c>
@@ -37635,38 +37651,38 @@
       <c r="AMI39"/>
       <c r="AMJ39"/>
     </row>
-    <row r="40" spans="1:1254" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:1254" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="10" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
-      <c r="B40" s="16">
+      <c r="B40" s="15">
         <v>3.4510000000000001</v>
       </c>
-      <c r="C40" s="20">
+      <c r="C40" s="19">
         <v>1</v>
       </c>
-      <c r="D40" s="17">
+      <c r="D40" s="16">
         <f t="shared" si="4"/>
         <v>24.157</v>
       </c>
-      <c r="E40" s="21" t="s">
-        <v>80</v>
+      <c r="E40" s="20" t="s">
+        <v>78</v>
       </c>
-      <c r="F40" s="21" t="s">
-        <v>81</v>
+      <c r="F40" s="20" t="s">
+        <v>79</v>
       </c>
-      <c r="G40" s="20" t="s">
+      <c r="G40" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H40" s="22"/>
-      <c r="I40" s="23"/>
-      <c r="J40" s="56" t="s">
-        <v>136</v>
+      <c r="H40" s="54"/>
+      <c r="I40" s="21"/>
+      <c r="J40" s="53" t="s">
+        <v>134</v>
       </c>
-      <c r="K40" s="56"/>
-      <c r="L40" s="56"/>
-      <c r="M40" s="56"/>
-      <c r="N40" s="56"/>
+      <c r="K40" s="53"/>
+      <c r="L40" s="53"/>
+      <c r="M40" s="53"/>
+      <c r="N40" s="53"/>
       <c r="O40" s="10">
         <v>7</v>
       </c>
@@ -38521,38 +38537,38 @@
       <c r="AMI40"/>
       <c r="AMJ40"/>
     </row>
-    <row r="41" spans="1:1254" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:1254" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="10" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
-      <c r="B41" s="16">
+      <c r="B41" s="15">
         <v>5.3</v>
       </c>
-      <c r="C41" s="20">
+      <c r="C41" s="19">
         <v>1</v>
       </c>
-      <c r="D41" s="17">
+      <c r="D41" s="16">
         <f t="shared" si="4"/>
         <v>26.5</v>
       </c>
-      <c r="E41" s="21" t="s">
-        <v>80</v>
+      <c r="E41" s="20" t="s">
+        <v>78</v>
       </c>
-      <c r="F41" s="21" t="s">
-        <v>135</v>
+      <c r="F41" s="20" t="s">
+        <v>133</v>
       </c>
-      <c r="G41" s="20" t="s">
+      <c r="G41" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H41" s="22"/>
-      <c r="I41" s="23"/>
-      <c r="J41" s="56" t="s">
-        <v>136</v>
+      <c r="H41" s="54"/>
+      <c r="I41" s="21"/>
+      <c r="J41" s="53" t="s">
+        <v>134</v>
       </c>
-      <c r="K41" s="56"/>
-      <c r="L41" s="56"/>
-      <c r="M41" s="56"/>
-      <c r="N41" s="56"/>
+      <c r="K41" s="53"/>
+      <c r="L41" s="53"/>
+      <c r="M41" s="53"/>
+      <c r="N41" s="53"/>
       <c r="O41" s="10">
         <v>5</v>
       </c>
@@ -39407,38 +39423,38 @@
       <c r="AMI41"/>
       <c r="AMJ41"/>
     </row>
-    <row r="42" spans="1:1254" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:1254" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="10" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
-      <c r="B42" s="16">
+      <c r="B42" s="15">
         <v>2.67</v>
       </c>
-      <c r="C42" s="20">
+      <c r="C42" s="19">
         <v>1</v>
       </c>
-      <c r="D42" s="17">
+      <c r="D42" s="16">
         <f t="shared" si="4"/>
         <v>8.01</v>
       </c>
-      <c r="E42" s="21" t="s">
-        <v>80</v>
+      <c r="E42" s="20" t="s">
+        <v>78</v>
       </c>
-      <c r="F42" s="21" t="s">
-        <v>137</v>
+      <c r="F42" s="20" t="s">
+        <v>135</v>
       </c>
-      <c r="G42" s="20" t="s">
+      <c r="G42" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H42" s="22"/>
-      <c r="I42" s="23"/>
-      <c r="J42" s="56" t="s">
-        <v>136</v>
+      <c r="H42" s="54"/>
+      <c r="I42" s="21"/>
+      <c r="J42" s="53" t="s">
+        <v>134</v>
       </c>
-      <c r="K42" s="56"/>
-      <c r="L42" s="56"/>
-      <c r="M42" s="56"/>
-      <c r="N42" s="56"/>
+      <c r="K42" s="53"/>
+      <c r="L42" s="53"/>
+      <c r="M42" s="53"/>
+      <c r="N42" s="53"/>
       <c r="O42" s="10">
         <v>3</v>
       </c>
@@ -40293,38 +40309,38 @@
       <c r="AMI42"/>
       <c r="AMJ42"/>
     </row>
-    <row r="43" spans="1:1254" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:1254" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="10" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
-      <c r="B43" s="16">
+      <c r="B43" s="15">
         <v>1.65</v>
       </c>
-      <c r="C43" s="20">
+      <c r="C43" s="19">
         <v>1</v>
       </c>
-      <c r="D43" s="17">
+      <c r="D43" s="16">
         <f t="shared" si="4"/>
         <v>4.9499999999999993</v>
       </c>
-      <c r="E43" s="21" t="s">
-        <v>80</v>
+      <c r="E43" s="20" t="s">
+        <v>78</v>
       </c>
-      <c r="F43" s="21" t="s">
-        <v>138</v>
+      <c r="F43" s="20" t="s">
+        <v>136</v>
       </c>
-      <c r="G43" s="20" t="s">
+      <c r="G43" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H43" s="22"/>
-      <c r="I43" s="23"/>
-      <c r="J43" s="56" t="s">
-        <v>136</v>
+      <c r="H43" s="54"/>
+      <c r="I43" s="21"/>
+      <c r="J43" s="53" t="s">
+        <v>134</v>
       </c>
-      <c r="K43" s="56"/>
-      <c r="L43" s="56"/>
-      <c r="M43" s="56"/>
-      <c r="N43" s="56"/>
+      <c r="K43" s="53"/>
+      <c r="L43" s="53"/>
+      <c r="M43" s="53"/>
+      <c r="N43" s="53"/>
       <c r="O43" s="10">
         <v>3</v>
       </c>
@@ -41179,38 +41195,38 @@
       <c r="AMI43"/>
       <c r="AMJ43"/>
     </row>
-    <row r="44" spans="1:1254" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:1254" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="10" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
-      <c r="B44" s="16">
+      <c r="B44" s="15">
         <v>2.1800000000000002</v>
       </c>
-      <c r="C44" s="20">
+      <c r="C44" s="19">
         <v>1</v>
       </c>
-      <c r="D44" s="17">
+      <c r="D44" s="16">
         <f t="shared" si="4"/>
         <v>13.080000000000002</v>
       </c>
-      <c r="E44" s="21" t="s">
-        <v>80</v>
+      <c r="E44" s="20" t="s">
+        <v>78</v>
       </c>
-      <c r="F44" s="21" t="s">
-        <v>139</v>
+      <c r="F44" s="20" t="s">
+        <v>137</v>
       </c>
-      <c r="G44" s="20" t="s">
+      <c r="G44" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H44" s="22"/>
-      <c r="I44" s="23"/>
-      <c r="J44" s="56" t="s">
-        <v>136</v>
+      <c r="H44" s="54"/>
+      <c r="I44" s="21"/>
+      <c r="J44" s="53" t="s">
+        <v>134</v>
       </c>
-      <c r="K44" s="56"/>
-      <c r="L44" s="56"/>
-      <c r="M44" s="56"/>
-      <c r="N44" s="56"/>
+      <c r="K44" s="53"/>
+      <c r="L44" s="53"/>
+      <c r="M44" s="53"/>
+      <c r="N44" s="53"/>
       <c r="O44" s="10">
         <v>6</v>
       </c>
@@ -42065,24 +42081,24 @@
       <c r="AMI44"/>
       <c r="AMJ44"/>
     </row>
-    <row r="45" spans="1:1254" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="60" t="s">
-        <v>83</v>
+    <row r="45" spans="1:1254" s="4" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="62" t="s">
+        <v>81</v>
       </c>
-      <c r="B45" s="60"/>
-      <c r="C45" s="60"/>
-      <c r="D45" s="60"/>
-      <c r="E45" s="60"/>
-      <c r="F45" s="60"/>
-      <c r="G45" s="60"/>
-      <c r="H45" s="60"/>
-      <c r="I45" s="60"/>
-      <c r="J45" s="60"/>
-      <c r="K45" s="60"/>
-      <c r="L45" s="60"/>
-      <c r="M45" s="60"/>
-      <c r="N45" s="60"/>
-      <c r="O45" s="60"/>
+      <c r="B45" s="62"/>
+      <c r="C45" s="62"/>
+      <c r="D45" s="62"/>
+      <c r="E45" s="62"/>
+      <c r="F45" s="62"/>
+      <c r="G45" s="62"/>
+      <c r="H45" s="62"/>
+      <c r="I45" s="62"/>
+      <c r="J45" s="62"/>
+      <c r="K45" s="62"/>
+      <c r="L45" s="62"/>
+      <c r="M45" s="62"/>
+      <c r="N45" s="62"/>
+      <c r="O45" s="62"/>
       <c r="P45"/>
       <c r="Q45"/>
       <c r="R45"/>
@@ -43323,39 +43339,39 @@
       <c r="AVE45"/>
       <c r="AVF45"/>
     </row>
-    <row r="46" spans="1:1254" ht="19.350000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:1254" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
-      <c r="B46" s="16">
+      <c r="B46" s="15">
         <v>13.54</v>
       </c>
-      <c r="C46" s="20">
+      <c r="C46" s="19">
         <v>1</v>
       </c>
-      <c r="D46" s="17">
+      <c r="D46" s="16">
         <f>B46*C46</f>
         <v>13.54</v>
       </c>
-      <c r="E46" s="21" t="s">
+      <c r="E46" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="F46" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="F46" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="G46" s="20" t="s">
+      <c r="G46" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H46" s="26" t="s">
-        <v>144</v>
+      <c r="H46" s="55" t="s">
+        <v>142</v>
       </c>
-      <c r="I46" s="41"/>
-      <c r="J46" s="57"/>
-      <c r="K46" s="57"/>
-      <c r="L46" s="57"/>
-      <c r="M46" s="57"/>
-      <c r="N46" s="57"/>
-      <c r="O46" s="57"/>
+      <c r="I46" s="36"/>
+      <c r="J46" s="48"/>
+      <c r="K46" s="48"/>
+      <c r="L46" s="48"/>
+      <c r="M46" s="48"/>
+      <c r="N46" s="48"/>
+      <c r="O46" s="48"/>
       <c r="FS46"/>
       <c r="FT46"/>
       <c r="FU46"/>
@@ -44207,39 +44223,39 @@
       <c r="AMI46"/>
       <c r="AMJ46"/>
     </row>
-    <row r="47" spans="1:1254" ht="19.350000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="31" t="s">
-        <v>84</v>
+    <row r="47" spans="1:1254" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="27" t="s">
+        <v>82</v>
       </c>
-      <c r="B47" s="15">
+      <c r="B47" s="14">
         <v>10.57</v>
       </c>
-      <c r="C47" s="32">
+      <c r="C47" s="28">
         <v>1</v>
       </c>
-      <c r="D47" s="17">
+      <c r="D47" s="16">
         <f t="shared" ref="D47:D63" si="5">B47*C47</f>
         <v>10.57</v>
       </c>
-      <c r="E47" s="34" t="s">
-        <v>20</v>
+      <c r="E47" s="30" t="s">
+        <v>19</v>
       </c>
-      <c r="F47" s="34" t="s">
-        <v>85</v>
+      <c r="F47" s="30" t="s">
+        <v>83</v>
       </c>
-      <c r="G47" s="20" t="s">
+      <c r="G47" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H47" s="26" t="s">
-        <v>144</v>
+      <c r="H47" s="55" t="s">
+        <v>142</v>
       </c>
-      <c r="I47" s="42"/>
-      <c r="J47" s="58"/>
-      <c r="K47" s="58"/>
-      <c r="L47" s="58"/>
-      <c r="M47" s="58"/>
-      <c r="N47" s="58"/>
-      <c r="O47" s="58"/>
+      <c r="I47" s="37"/>
+      <c r="J47" s="50"/>
+      <c r="K47" s="50"/>
+      <c r="L47" s="50"/>
+      <c r="M47" s="50"/>
+      <c r="N47" s="50"/>
+      <c r="O47" s="50"/>
       <c r="FS47"/>
       <c r="FT47"/>
       <c r="FU47"/>
@@ -45091,41 +45107,41 @@
       <c r="AMI47"/>
       <c r="AMJ47"/>
     </row>
-    <row r="48" spans="1:1254" ht="19.350000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="43" t="s">
-        <v>87</v>
+    <row r="48" spans="1:1254" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="38" t="s">
+        <v>85</v>
       </c>
-      <c r="B48" s="15">
+      <c r="B48" s="14">
         <v>73.180000000000007</v>
       </c>
-      <c r="C48" s="32">
+      <c r="C48" s="28">
         <v>1</v>
       </c>
-      <c r="D48" s="17">
+      <c r="D48" s="16">
         <f t="shared" si="5"/>
         <v>73.180000000000007</v>
       </c>
-      <c r="E48" s="34" t="s">
-        <v>88</v>
+      <c r="E48" s="30" t="s">
+        <v>86</v>
       </c>
-      <c r="F48" s="34" t="s">
-        <v>89</v>
+      <c r="F48" s="30" t="s">
+        <v>87</v>
       </c>
-      <c r="G48" s="20" t="s">
+      <c r="G48" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H48" s="26" t="s">
-        <v>144</v>
+      <c r="H48" s="55" t="s">
+        <v>142</v>
       </c>
-      <c r="I48" s="42"/>
-      <c r="J48" s="57" t="s">
-        <v>92</v>
+      <c r="I48" s="37"/>
+      <c r="J48" s="48" t="s">
+        <v>90</v>
       </c>
-      <c r="K48" s="57"/>
-      <c r="L48" s="57"/>
-      <c r="M48" s="57"/>
-      <c r="N48" s="57"/>
-      <c r="O48" s="57"/>
+      <c r="K48" s="48"/>
+      <c r="L48" s="48"/>
+      <c r="M48" s="48"/>
+      <c r="N48" s="48"/>
+      <c r="O48" s="48"/>
       <c r="FS48"/>
       <c r="FT48"/>
       <c r="FU48"/>
@@ -45977,41 +45993,41 @@
       <c r="AMI48"/>
       <c r="AMJ48"/>
     </row>
-    <row r="49" spans="1:1254" ht="19.350000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="43" t="s">
-        <v>90</v>
+    <row r="49" spans="1:1254" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="38" t="s">
+        <v>88</v>
       </c>
-      <c r="B49" s="15">
+      <c r="B49" s="14">
         <v>17.399999999999999</v>
       </c>
-      <c r="C49" s="32">
+      <c r="C49" s="28">
         <v>1</v>
       </c>
-      <c r="D49" s="17">
+      <c r="D49" s="16">
         <f t="shared" si="5"/>
         <v>17.399999999999999</v>
       </c>
-      <c r="E49" s="34" t="s">
-        <v>20</v>
+      <c r="E49" s="30" t="s">
+        <v>19</v>
       </c>
-      <c r="F49" s="34" t="s">
+      <c r="F49" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="G49" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="H49" s="55" t="s">
+        <v>142</v>
+      </c>
+      <c r="I49" s="34"/>
+      <c r="J49" s="48" t="s">
         <v>91</v>
       </c>
-      <c r="G49" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="H49" s="26" t="s">
-        <v>144</v>
-      </c>
-      <c r="I49" s="39"/>
-      <c r="J49" s="57" t="s">
-        <v>93</v>
-      </c>
-      <c r="K49" s="57"/>
-      <c r="L49" s="57"/>
-      <c r="M49" s="57"/>
-      <c r="N49" s="57"/>
-      <c r="O49" s="57"/>
+      <c r="K49" s="48"/>
+      <c r="L49" s="48"/>
+      <c r="M49" s="48"/>
+      <c r="N49" s="48"/>
+      <c r="O49" s="48"/>
       <c r="FS49"/>
       <c r="FT49"/>
       <c r="FU49"/>
@@ -46863,39 +46879,39 @@
       <c r="AMI49"/>
       <c r="AMJ49"/>
     </row>
-    <row r="50" spans="1:1254" ht="19.350000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="31" t="s">
-        <v>94</v>
+    <row r="50" spans="1:1254" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="27" t="s">
+        <v>92</v>
       </c>
-      <c r="B50" s="15">
+      <c r="B50" s="14">
         <v>2.54</v>
       </c>
-      <c r="C50" s="32">
+      <c r="C50" s="28">
         <v>2</v>
       </c>
-      <c r="D50" s="17">
+      <c r="D50" s="16">
         <f t="shared" si="5"/>
         <v>5.08</v>
       </c>
-      <c r="E50" s="34" t="s">
-        <v>20</v>
+      <c r="E50" s="30" t="s">
+        <v>19</v>
       </c>
-      <c r="F50" s="34" t="s">
-        <v>95</v>
+      <c r="F50" s="30" t="s">
+        <v>93</v>
       </c>
-      <c r="G50" s="20" t="s">
+      <c r="G50" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H50" s="26" t="s">
-        <v>144</v>
+      <c r="H50" s="55" t="s">
+        <v>142</v>
       </c>
-      <c r="I50" s="39"/>
-      <c r="J50" s="57"/>
-      <c r="K50" s="57"/>
-      <c r="L50" s="57"/>
-      <c r="M50" s="57"/>
-      <c r="N50" s="57"/>
-      <c r="O50" s="57"/>
+      <c r="I50" s="34"/>
+      <c r="J50" s="48"/>
+      <c r="K50" s="48"/>
+      <c r="L50" s="48"/>
+      <c r="M50" s="48"/>
+      <c r="N50" s="48"/>
+      <c r="O50" s="48"/>
       <c r="FS50"/>
       <c r="FT50"/>
       <c r="FU50"/>
@@ -47747,41 +47763,41 @@
       <c r="AMI50"/>
       <c r="AMJ50"/>
     </row>
-    <row r="51" spans="1:1254" ht="19.350000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="43" t="s">
-        <v>96</v>
+    <row r="51" spans="1:1254" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="38" t="s">
+        <v>94</v>
       </c>
-      <c r="B51" s="15">
+      <c r="B51" s="14">
         <v>18.95</v>
       </c>
-      <c r="C51" s="32">
+      <c r="C51" s="28">
         <v>1</v>
       </c>
-      <c r="D51" s="17">
+      <c r="D51" s="16">
         <f t="shared" si="5"/>
         <v>18.95</v>
       </c>
-      <c r="E51" s="34" t="s">
-        <v>88</v>
+      <c r="E51" s="30" t="s">
+        <v>86</v>
       </c>
-      <c r="F51" s="34" t="s">
-        <v>97</v>
+      <c r="F51" s="30" t="s">
+        <v>95</v>
       </c>
-      <c r="G51" s="20" t="s">
+      <c r="G51" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H51" s="26" t="s">
-        <v>144</v>
+      <c r="H51" s="55" t="s">
+        <v>142</v>
       </c>
-      <c r="I51" s="39"/>
-      <c r="J51" s="57" t="s">
-        <v>98</v>
+      <c r="I51" s="34"/>
+      <c r="J51" s="48" t="s">
+        <v>96</v>
       </c>
-      <c r="K51" s="57"/>
-      <c r="L51" s="57"/>
-      <c r="M51" s="57"/>
-      <c r="N51" s="57"/>
-      <c r="O51" s="57"/>
+      <c r="K51" s="48"/>
+      <c r="L51" s="48"/>
+      <c r="M51" s="48"/>
+      <c r="N51" s="48"/>
+      <c r="O51" s="48"/>
       <c r="FS51"/>
       <c r="FT51"/>
       <c r="FU51"/>
@@ -48633,39 +48649,39 @@
       <c r="AMI51"/>
       <c r="AMJ51"/>
     </row>
-    <row r="52" spans="1:1254" ht="19.350000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="43" t="s">
-        <v>87</v>
+    <row r="52" spans="1:1254" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="38" t="s">
+        <v>85</v>
       </c>
-      <c r="B52" s="15">
+      <c r="B52" s="14">
         <v>73.180000000000007</v>
       </c>
-      <c r="C52" s="32">
+      <c r="C52" s="28">
         <v>1</v>
       </c>
-      <c r="D52" s="17">
+      <c r="D52" s="16">
         <f t="shared" si="5"/>
         <v>73.180000000000007</v>
       </c>
-      <c r="E52" s="34" t="s">
-        <v>88</v>
+      <c r="E52" s="30" t="s">
+        <v>86</v>
       </c>
-      <c r="F52" s="34" t="s">
-        <v>89</v>
+      <c r="F52" s="30" t="s">
+        <v>87</v>
       </c>
-      <c r="G52" s="20" t="s">
+      <c r="G52" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H52" s="26" t="s">
-        <v>144</v>
+      <c r="H52" s="55" t="s">
+        <v>142</v>
       </c>
-      <c r="I52" s="42"/>
-      <c r="J52" s="57"/>
-      <c r="K52" s="57"/>
-      <c r="L52" s="57"/>
-      <c r="M52" s="57"/>
-      <c r="N52" s="57"/>
-      <c r="O52" s="57"/>
+      <c r="I52" s="37"/>
+      <c r="J52" s="48"/>
+      <c r="K52" s="48"/>
+      <c r="L52" s="48"/>
+      <c r="M52" s="48"/>
+      <c r="N52" s="48"/>
+      <c r="O52" s="48"/>
       <c r="FS52"/>
       <c r="FT52"/>
       <c r="FU52"/>
@@ -49517,39 +49533,39 @@
       <c r="AMI52"/>
       <c r="AMJ52"/>
     </row>
-    <row r="53" spans="1:1254" ht="19.350000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="31" t="s">
-        <v>99</v>
+    <row r="53" spans="1:1254" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="27" t="s">
+        <v>97</v>
       </c>
-      <c r="B53" s="15">
+      <c r="B53" s="14">
         <v>2.81</v>
       </c>
-      <c r="C53" s="32">
+      <c r="C53" s="28">
         <v>1</v>
       </c>
-      <c r="D53" s="17">
+      <c r="D53" s="16">
         <f t="shared" si="5"/>
         <v>2.81</v>
       </c>
-      <c r="E53" s="34" t="s">
-        <v>20</v>
+      <c r="E53" s="30" t="s">
+        <v>19</v>
       </c>
-      <c r="F53" s="34" t="s">
-        <v>100</v>
+      <c r="F53" s="30" t="s">
+        <v>98</v>
       </c>
-      <c r="G53" s="20" t="s">
+      <c r="G53" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H53" s="26" t="s">
-        <v>144</v>
+      <c r="H53" s="55" t="s">
+        <v>142</v>
       </c>
-      <c r="I53" s="39"/>
-      <c r="J53" s="57"/>
-      <c r="K53" s="57"/>
-      <c r="L53" s="57"/>
-      <c r="M53" s="57"/>
-      <c r="N53" s="57"/>
-      <c r="O53" s="57"/>
+      <c r="I53" s="34"/>
+      <c r="J53" s="48"/>
+      <c r="K53" s="48"/>
+      <c r="L53" s="48"/>
+      <c r="M53" s="48"/>
+      <c r="N53" s="48"/>
+      <c r="O53" s="48"/>
       <c r="FS53"/>
       <c r="FT53"/>
       <c r="FU53"/>
@@ -50401,39 +50417,39 @@
       <c r="AMI53"/>
       <c r="AMJ53"/>
     </row>
-    <row r="54" spans="1:1254" ht="19.350000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="31" t="s">
-        <v>101</v>
+    <row r="54" spans="1:1254" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="27" t="s">
+        <v>99</v>
       </c>
-      <c r="B54" s="15">
+      <c r="B54" s="14">
         <v>3.69</v>
       </c>
-      <c r="C54" s="32">
+      <c r="C54" s="28">
         <v>1</v>
       </c>
-      <c r="D54" s="17">
+      <c r="D54" s="16">
         <f t="shared" si="5"/>
         <v>3.69</v>
       </c>
-      <c r="E54" s="34" t="s">
-        <v>20</v>
+      <c r="E54" s="30" t="s">
+        <v>19</v>
       </c>
-      <c r="F54" s="34" t="s">
-        <v>102</v>
+      <c r="F54" s="30" t="s">
+        <v>100</v>
       </c>
-      <c r="G54" s="20" t="s">
+      <c r="G54" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H54" s="26" t="s">
-        <v>144</v>
+      <c r="H54" s="55" t="s">
+        <v>142</v>
       </c>
-      <c r="I54" s="39"/>
-      <c r="J54" s="57"/>
-      <c r="K54" s="57"/>
-      <c r="L54" s="57"/>
-      <c r="M54" s="57"/>
-      <c r="N54" s="57"/>
-      <c r="O54" s="57"/>
+      <c r="I54" s="34"/>
+      <c r="J54" s="48"/>
+      <c r="K54" s="48"/>
+      <c r="L54" s="48"/>
+      <c r="M54" s="48"/>
+      <c r="N54" s="48"/>
+      <c r="O54" s="48"/>
       <c r="FS54"/>
       <c r="FT54"/>
       <c r="FU54"/>
@@ -51285,41 +51301,41 @@
       <c r="AMI54"/>
       <c r="AMJ54"/>
     </row>
-    <row r="55" spans="1:1254" ht="19.350000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="31" t="s">
-        <v>103</v>
+    <row r="55" spans="1:1254" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="27" t="s">
+        <v>101</v>
       </c>
-      <c r="B55" s="15">
+      <c r="B55" s="14">
         <v>15.32</v>
       </c>
-      <c r="C55" s="32">
+      <c r="C55" s="28">
         <v>1</v>
       </c>
-      <c r="D55" s="17">
+      <c r="D55" s="16">
         <f t="shared" si="5"/>
         <v>15.32</v>
       </c>
-      <c r="E55" s="34" t="s">
-        <v>88</v>
+      <c r="E55" s="30" t="s">
+        <v>86</v>
       </c>
-      <c r="F55" s="44" t="s">
-        <v>104</v>
+      <c r="F55" s="39" t="s">
+        <v>102</v>
       </c>
-      <c r="G55" s="20" t="s">
+      <c r="G55" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H55" s="26" t="s">
-        <v>144</v>
+      <c r="H55" s="55" t="s">
+        <v>142</v>
       </c>
-      <c r="I55" s="39"/>
-      <c r="J55" s="57" t="s">
-        <v>107</v>
+      <c r="I55" s="34"/>
+      <c r="J55" s="48" t="s">
+        <v>105</v>
       </c>
-      <c r="K55" s="57"/>
-      <c r="L55" s="57"/>
-      <c r="M55" s="57"/>
-      <c r="N55" s="57"/>
-      <c r="O55" s="57"/>
+      <c r="K55" s="48"/>
+      <c r="L55" s="48"/>
+      <c r="M55" s="48"/>
+      <c r="N55" s="48"/>
+      <c r="O55" s="48"/>
       <c r="FS55"/>
       <c r="FT55"/>
       <c r="FU55"/>
@@ -52171,41 +52187,41 @@
       <c r="AMI55"/>
       <c r="AMJ55"/>
     </row>
-    <row r="56" spans="1:1254" ht="19.350000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="31" t="s">
-        <v>105</v>
+    <row r="56" spans="1:1254" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="27" t="s">
+        <v>103</v>
       </c>
-      <c r="B56" s="15">
+      <c r="B56" s="14">
         <v>56.31</v>
       </c>
-      <c r="C56" s="32">
+      <c r="C56" s="28">
         <v>1</v>
       </c>
-      <c r="D56" s="17">
+      <c r="D56" s="16">
         <f t="shared" si="5"/>
         <v>56.31</v>
       </c>
-      <c r="E56" s="34" t="s">
-        <v>88</v>
+      <c r="E56" s="30" t="s">
+        <v>86</v>
       </c>
-      <c r="F56" s="34" t="s">
+      <c r="F56" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="G56" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="H56" s="55" t="s">
+        <v>142</v>
+      </c>
+      <c r="I56" s="34"/>
+      <c r="J56" s="48" t="s">
         <v>106</v>
       </c>
-      <c r="G56" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="H56" s="26" t="s">
-        <v>144</v>
-      </c>
-      <c r="I56" s="39"/>
-      <c r="J56" s="57" t="s">
-        <v>108</v>
-      </c>
-      <c r="K56" s="57"/>
-      <c r="L56" s="57"/>
-      <c r="M56" s="57"/>
-      <c r="N56" s="57"/>
-      <c r="O56" s="57"/>
+      <c r="K56" s="48"/>
+      <c r="L56" s="48"/>
+      <c r="M56" s="48"/>
+      <c r="N56" s="48"/>
+      <c r="O56" s="48"/>
       <c r="FS56"/>
       <c r="FT56"/>
       <c r="FU56"/>
@@ -53057,39 +53073,39 @@
       <c r="AMI56"/>
       <c r="AMJ56"/>
     </row>
-    <row r="57" spans="1:1254" ht="19.350000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="43" t="s">
-        <v>90</v>
+    <row r="57" spans="1:1254" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="38" t="s">
+        <v>88</v>
       </c>
-      <c r="B57" s="15">
+      <c r="B57" s="14">
         <v>17.399999999999999</v>
       </c>
-      <c r="C57" s="32">
+      <c r="C57" s="28">
         <v>1</v>
       </c>
-      <c r="D57" s="17">
+      <c r="D57" s="16">
         <f t="shared" si="5"/>
         <v>17.399999999999999</v>
       </c>
-      <c r="E57" s="34" t="s">
-        <v>20</v>
+      <c r="E57" s="30" t="s">
+        <v>19</v>
       </c>
-      <c r="F57" s="34" t="s">
-        <v>91</v>
+      <c r="F57" s="30" t="s">
+        <v>89</v>
       </c>
-      <c r="G57" s="20" t="s">
+      <c r="G57" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H57" s="26" t="s">
-        <v>144</v>
+      <c r="H57" s="55" t="s">
+        <v>142</v>
       </c>
-      <c r="I57" s="39"/>
-      <c r="J57" s="57"/>
-      <c r="K57" s="57"/>
-      <c r="L57" s="57"/>
-      <c r="M57" s="57"/>
-      <c r="N57" s="57"/>
-      <c r="O57" s="57"/>
+      <c r="I57" s="34"/>
+      <c r="J57" s="48"/>
+      <c r="K57" s="48"/>
+      <c r="L57" s="48"/>
+      <c r="M57" s="48"/>
+      <c r="N57" s="48"/>
+      <c r="O57" s="48"/>
       <c r="FS57"/>
       <c r="FT57"/>
       <c r="FU57"/>
@@ -53941,39 +53957,39 @@
       <c r="AMI57"/>
       <c r="AMJ57"/>
     </row>
-    <row r="58" spans="1:1254" ht="19.350000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="31" t="s">
-        <v>109</v>
+    <row r="58" spans="1:1254" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="27" t="s">
+        <v>107</v>
       </c>
-      <c r="B58" s="15">
+      <c r="B58" s="14">
         <v>66.39</v>
       </c>
-      <c r="C58" s="32">
+      <c r="C58" s="28">
         <v>1</v>
       </c>
-      <c r="D58" s="17">
+      <c r="D58" s="16">
         <f t="shared" si="5"/>
         <v>66.39</v>
       </c>
-      <c r="E58" s="34" t="s">
-        <v>20</v>
+      <c r="E58" s="30" t="s">
+        <v>19</v>
       </c>
-      <c r="F58" s="34" t="s">
-        <v>110</v>
+      <c r="F58" s="30" t="s">
+        <v>108</v>
       </c>
-      <c r="G58" s="20" t="s">
+      <c r="G58" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H58" s="26" t="s">
-        <v>144</v>
+      <c r="H58" s="55" t="s">
+        <v>142</v>
       </c>
-      <c r="I58" s="39"/>
-      <c r="J58" s="57"/>
-      <c r="K58" s="57"/>
-      <c r="L58" s="57"/>
-      <c r="M58" s="57"/>
-      <c r="N58" s="57"/>
-      <c r="O58" s="57"/>
+      <c r="I58" s="34"/>
+      <c r="J58" s="48"/>
+      <c r="K58" s="48"/>
+      <c r="L58" s="48"/>
+      <c r="M58" s="48"/>
+      <c r="N58" s="48"/>
+      <c r="O58" s="48"/>
       <c r="FS58"/>
       <c r="FT58"/>
       <c r="FU58"/>
@@ -54825,39 +54841,39 @@
       <c r="AMI58"/>
       <c r="AMJ58"/>
     </row>
-    <row r="59" spans="1:1254" ht="19.350000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="31" t="s">
-        <v>111</v>
+    <row r="59" spans="1:1254" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="27" t="s">
+        <v>109</v>
       </c>
-      <c r="B59" s="15">
+      <c r="B59" s="14">
         <v>16.98</v>
       </c>
-      <c r="C59" s="32">
+      <c r="C59" s="28">
         <v>2</v>
       </c>
-      <c r="D59" s="17">
+      <c r="D59" s="16">
         <f t="shared" si="5"/>
         <v>33.96</v>
       </c>
-      <c r="E59" s="34" t="s">
-        <v>88</v>
+      <c r="E59" s="30" t="s">
+        <v>86</v>
       </c>
-      <c r="F59" s="34" t="s">
-        <v>112</v>
+      <c r="F59" s="30" t="s">
+        <v>110</v>
       </c>
-      <c r="G59" s="20" t="s">
+      <c r="G59" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H59" s="26" t="s">
-        <v>144</v>
+      <c r="H59" s="55" t="s">
+        <v>142</v>
       </c>
-      <c r="I59" s="39"/>
-      <c r="J59" s="57"/>
-      <c r="K59" s="57"/>
-      <c r="L59" s="57"/>
-      <c r="M59" s="57"/>
-      <c r="N59" s="57"/>
-      <c r="O59" s="57"/>
+      <c r="I59" s="34"/>
+      <c r="J59" s="48"/>
+      <c r="K59" s="48"/>
+      <c r="L59" s="48"/>
+      <c r="M59" s="48"/>
+      <c r="N59" s="48"/>
+      <c r="O59" s="48"/>
       <c r="FS59"/>
       <c r="FT59"/>
       <c r="FU59"/>
@@ -55709,39 +55725,39 @@
       <c r="AMI59"/>
       <c r="AMJ59"/>
     </row>
-    <row r="60" spans="1:1254" ht="19.350000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="43" t="s">
-        <v>113</v>
+    <row r="60" spans="1:1254" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="38" t="s">
+        <v>111</v>
       </c>
-      <c r="B60" s="15">
+      <c r="B60" s="14">
         <v>24.85</v>
       </c>
-      <c r="C60" s="32">
+      <c r="C60" s="28">
         <v>1</v>
       </c>
-      <c r="D60" s="17">
+      <c r="D60" s="16">
         <f t="shared" si="5"/>
         <v>24.85</v>
       </c>
-      <c r="E60" s="34" t="s">
-        <v>20</v>
+      <c r="E60" s="30" t="s">
+        <v>19</v>
       </c>
-      <c r="F60" s="34" t="s">
-        <v>114</v>
+      <c r="F60" s="30" t="s">
+        <v>112</v>
       </c>
-      <c r="G60" s="20" t="s">
+      <c r="G60" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H60" s="26" t="s">
-        <v>144</v>
+      <c r="H60" s="55" t="s">
+        <v>142</v>
       </c>
-      <c r="I60" s="39"/>
-      <c r="J60" s="57"/>
-      <c r="K60" s="57"/>
-      <c r="L60" s="57"/>
-      <c r="M60" s="57"/>
-      <c r="N60" s="57"/>
-      <c r="O60" s="57"/>
+      <c r="I60" s="34"/>
+      <c r="J60" s="48"/>
+      <c r="K60" s="48"/>
+      <c r="L60" s="48"/>
+      <c r="M60" s="48"/>
+      <c r="N60" s="48"/>
+      <c r="O60" s="48"/>
       <c r="FS60"/>
       <c r="FT60"/>
       <c r="FU60"/>
@@ -56593,39 +56609,39 @@
       <c r="AMI60"/>
       <c r="AMJ60"/>
     </row>
-    <row r="61" spans="1:1254" ht="19.350000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="43" t="s">
-        <v>115</v>
+    <row r="61" spans="1:1254" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="38" t="s">
+        <v>113</v>
       </c>
-      <c r="B61" s="15">
+      <c r="B61" s="14">
         <v>16.2</v>
       </c>
-      <c r="C61" s="32">
+      <c r="C61" s="28">
         <v>1</v>
       </c>
-      <c r="D61" s="17">
+      <c r="D61" s="16">
         <f t="shared" si="5"/>
         <v>16.2</v>
       </c>
-      <c r="E61" s="34" t="s">
-        <v>20</v>
+      <c r="E61" s="30" t="s">
+        <v>19</v>
       </c>
-      <c r="F61" s="34" t="s">
-        <v>116</v>
+      <c r="F61" s="30" t="s">
+        <v>114</v>
       </c>
-      <c r="G61" s="20" t="s">
+      <c r="G61" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H61" s="26" t="s">
-        <v>144</v>
+      <c r="H61" s="55" t="s">
+        <v>142</v>
       </c>
-      <c r="I61" s="39"/>
-      <c r="J61" s="57"/>
-      <c r="K61" s="57"/>
-      <c r="L61" s="57"/>
-      <c r="M61" s="57"/>
-      <c r="N61" s="57"/>
-      <c r="O61" s="57"/>
+      <c r="I61" s="34"/>
+      <c r="J61" s="48"/>
+      <c r="K61" s="48"/>
+      <c r="L61" s="48"/>
+      <c r="M61" s="48"/>
+      <c r="N61" s="48"/>
+      <c r="O61" s="48"/>
       <c r="FS61"/>
       <c r="FT61"/>
       <c r="FU61"/>
@@ -57477,39 +57493,39 @@
       <c r="AMI61"/>
       <c r="AMJ61"/>
     </row>
-    <row r="62" spans="1:1254" ht="19.350000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="31" t="s">
-        <v>129</v>
+    <row r="62" spans="1:1254" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="27" t="s">
+        <v>127</v>
       </c>
-      <c r="B62" s="15">
+      <c r="B62" s="14">
         <v>49.39</v>
       </c>
-      <c r="C62" s="32">
+      <c r="C62" s="28">
         <v>1</v>
       </c>
-      <c r="D62" s="17">
+      <c r="D62" s="16">
         <f t="shared" si="5"/>
         <v>49.39</v>
       </c>
-      <c r="E62" s="34" t="s">
-        <v>20</v>
+      <c r="E62" s="30" t="s">
+        <v>19</v>
       </c>
-      <c r="F62" s="34" t="s">
-        <v>130</v>
+      <c r="F62" s="30" t="s">
+        <v>128</v>
       </c>
-      <c r="G62" s="20" t="s">
+      <c r="G62" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H62" s="26" t="s">
-        <v>144</v>
+      <c r="H62" s="55" t="s">
+        <v>142</v>
       </c>
-      <c r="I62" s="39"/>
-      <c r="J62" s="57"/>
-      <c r="K62" s="57"/>
-      <c r="L62" s="57"/>
-      <c r="M62" s="57"/>
-      <c r="N62" s="57"/>
-      <c r="O62" s="57"/>
+      <c r="I62" s="34"/>
+      <c r="J62" s="48"/>
+      <c r="K62" s="48"/>
+      <c r="L62" s="48"/>
+      <c r="M62" s="48"/>
+      <c r="N62" s="48"/>
+      <c r="O62" s="48"/>
       <c r="FS62"/>
       <c r="FT62"/>
       <c r="FU62"/>
@@ -58361,39 +58377,39 @@
       <c r="AMI62"/>
       <c r="AMJ62"/>
     </row>
-    <row r="63" spans="1:1254" ht="19.350000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="31" t="s">
-        <v>131</v>
+    <row r="63" spans="1:1254" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="27" t="s">
+        <v>129</v>
       </c>
-      <c r="B63" s="15">
+      <c r="B63" s="14">
         <v>131.82</v>
       </c>
-      <c r="C63" s="32">
+      <c r="C63" s="28">
         <v>1</v>
       </c>
-      <c r="D63" s="17">
+      <c r="D63" s="16">
         <f t="shared" si="5"/>
         <v>131.82</v>
       </c>
-      <c r="E63" s="34" t="s">
-        <v>78</v>
+      <c r="E63" s="30" t="s">
+        <v>76</v>
       </c>
-      <c r="F63" s="34" t="s">
-        <v>86</v>
+      <c r="F63" s="30" t="s">
+        <v>84</v>
       </c>
-      <c r="G63" s="20" t="s">
+      <c r="G63" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H63" s="26" t="s">
-        <v>144</v>
+      <c r="H63" s="55" t="s">
+        <v>142</v>
       </c>
-      <c r="I63" s="39"/>
-      <c r="J63" s="57"/>
-      <c r="K63" s="57"/>
-      <c r="L63" s="57"/>
-      <c r="M63" s="57"/>
-      <c r="N63" s="57"/>
-      <c r="O63" s="57"/>
+      <c r="I63" s="34"/>
+      <c r="J63" s="48"/>
+      <c r="K63" s="48"/>
+      <c r="L63" s="48"/>
+      <c r="M63" s="48"/>
+      <c r="N63" s="48"/>
+      <c r="O63" s="48"/>
       <c r="FS63"/>
       <c r="FT63"/>
       <c r="FU63"/>
@@ -59245,24 +59261,24 @@
       <c r="AMI63"/>
       <c r="AMJ63"/>
     </row>
-    <row r="64" spans="1:1254" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="60" t="s">
-        <v>72</v>
+    <row r="64" spans="1:1254" s="4" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="62" t="s">
+        <v>71</v>
       </c>
-      <c r="B64" s="60"/>
-      <c r="C64" s="60"/>
-      <c r="D64" s="60"/>
-      <c r="E64" s="60"/>
-      <c r="F64" s="60"/>
-      <c r="G64" s="60"/>
-      <c r="H64" s="60"/>
-      <c r="I64" s="60"/>
-      <c r="J64" s="60"/>
-      <c r="K64" s="60"/>
-      <c r="L64" s="60"/>
-      <c r="M64" s="60"/>
-      <c r="N64" s="60"/>
-      <c r="O64" s="60"/>
+      <c r="B64" s="62"/>
+      <c r="C64" s="62"/>
+      <c r="D64" s="62"/>
+      <c r="E64" s="62"/>
+      <c r="F64" s="62"/>
+      <c r="G64" s="62"/>
+      <c r="H64" s="62"/>
+      <c r="I64" s="62"/>
+      <c r="J64" s="62"/>
+      <c r="K64" s="62"/>
+      <c r="L64" s="62"/>
+      <c r="M64" s="62"/>
+      <c r="N64" s="62"/>
+      <c r="O64" s="62"/>
       <c r="P64"/>
       <c r="Q64"/>
       <c r="R64"/>
@@ -60503,24 +60519,24 @@
       <c r="AVE64"/>
       <c r="AVF64"/>
     </row>
-    <row r="65" spans="1:1254" s="5" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="45"/>
-      <c r="B65" s="46"/>
-      <c r="C65" s="47"/>
-      <c r="D65" s="48"/>
-      <c r="E65" s="33"/>
-      <c r="F65" s="33"/>
-      <c r="G65" s="20" t="s">
+    <row r="65" spans="1:1254" s="5" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="40"/>
+      <c r="B65" s="41"/>
+      <c r="C65" s="42"/>
+      <c r="D65" s="43"/>
+      <c r="E65" s="29"/>
+      <c r="F65" s="29"/>
+      <c r="G65" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H65" s="49"/>
-      <c r="I65" s="45"/>
-      <c r="J65" s="59"/>
-      <c r="K65" s="59"/>
-      <c r="L65" s="59"/>
-      <c r="M65" s="59"/>
-      <c r="N65" s="59"/>
-      <c r="O65" s="59"/>
+      <c r="H65" s="44"/>
+      <c r="I65" s="40"/>
+      <c r="J65" s="52"/>
+      <c r="K65" s="52"/>
+      <c r="L65" s="52"/>
+      <c r="M65" s="52"/>
+      <c r="N65" s="52"/>
+      <c r="O65" s="52"/>
       <c r="P65"/>
       <c r="Q65"/>
       <c r="R65"/>
@@ -61761,24 +61777,24 @@
       <c r="AVE65"/>
       <c r="AVF65"/>
     </row>
-    <row r="66" spans="1:1254" s="5" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="45"/>
-      <c r="B66" s="46"/>
-      <c r="C66" s="47"/>
-      <c r="D66" s="48"/>
-      <c r="E66" s="33"/>
-      <c r="F66" s="33"/>
-      <c r="G66" s="20" t="s">
+    <row r="66" spans="1:1254" s="5" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="40"/>
+      <c r="B66" s="41"/>
+      <c r="C66" s="42"/>
+      <c r="D66" s="43"/>
+      <c r="E66" s="29"/>
+      <c r="F66" s="29"/>
+      <c r="G66" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H66" s="49"/>
-      <c r="I66" s="45"/>
-      <c r="J66" s="59"/>
-      <c r="K66" s="59"/>
-      <c r="L66" s="59"/>
-      <c r="M66" s="59"/>
-      <c r="N66" s="59"/>
-      <c r="O66" s="59"/>
+      <c r="H66" s="44"/>
+      <c r="I66" s="40"/>
+      <c r="J66" s="52"/>
+      <c r="K66" s="52"/>
+      <c r="L66" s="52"/>
+      <c r="M66" s="52"/>
+      <c r="N66" s="52"/>
+      <c r="O66" s="52"/>
       <c r="P66"/>
       <c r="Q66"/>
       <c r="R66"/>
@@ -63020,23 +63036,23 @@
       <c r="AVF66"/>
     </row>
     <row r="67" spans="1:1254" ht="19.350000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="60" t="s">
-        <v>73</v>
+      <c r="A67" s="62" t="s">
+        <v>72</v>
       </c>
-      <c r="B67" s="60"/>
-      <c r="C67" s="60"/>
-      <c r="D67" s="60"/>
-      <c r="E67" s="60"/>
-      <c r="F67" s="60"/>
-      <c r="G67" s="60"/>
-      <c r="H67" s="60"/>
-      <c r="I67" s="60"/>
-      <c r="J67" s="60"/>
-      <c r="K67" s="60"/>
-      <c r="L67" s="60"/>
-      <c r="M67" s="60"/>
-      <c r="N67" s="60"/>
-      <c r="O67" s="60"/>
+      <c r="B67" s="62"/>
+      <c r="C67" s="62"/>
+      <c r="D67" s="62"/>
+      <c r="E67" s="62"/>
+      <c r="F67" s="62"/>
+      <c r="G67" s="62"/>
+      <c r="H67" s="62"/>
+      <c r="I67" s="62"/>
+      <c r="J67" s="62"/>
+      <c r="K67" s="62"/>
+      <c r="L67" s="62"/>
+      <c r="M67" s="62"/>
+      <c r="N67" s="62"/>
+      <c r="O67" s="62"/>
       <c r="FS67"/>
       <c r="FT67"/>
       <c r="FU67"/>
@@ -63889,38 +63905,38 @@
       <c r="AMJ67"/>
     </row>
     <row r="68" spans="1:1254" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="50" t="s">
-        <v>77</v>
+      <c r="A68" s="45" t="s">
+        <v>75</v>
       </c>
-      <c r="B68" s="14">
+      <c r="B68" s="13">
         <v>28.8</v>
       </c>
-      <c r="C68" s="29">
+      <c r="C68" s="26">
         <v>1</v>
       </c>
-      <c r="D68" s="17">
+      <c r="D68" s="16">
         <f>B68*C68</f>
         <v>28.8</v>
       </c>
-      <c r="E68" s="51" t="s">
-        <v>78</v>
+      <c r="E68" s="46" t="s">
+        <v>76</v>
       </c>
-      <c r="F68" s="25" t="s">
-        <v>133</v>
+      <c r="F68" s="23" t="s">
+        <v>131</v>
       </c>
-      <c r="G68" s="20" t="s">
+      <c r="G68" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H68" s="26" t="s">
-        <v>144</v>
+      <c r="H68" s="55" t="s">
+        <v>142</v>
       </c>
-      <c r="I68" s="52"/>
-      <c r="J68" s="58"/>
-      <c r="K68" s="58"/>
-      <c r="L68" s="58"/>
-      <c r="M68" s="58"/>
-      <c r="N68" s="58"/>
-      <c r="O68" s="58"/>
+      <c r="I68" s="47"/>
+      <c r="J68" s="50"/>
+      <c r="K68" s="50"/>
+      <c r="L68" s="50"/>
+      <c r="M68" s="50"/>
+      <c r="N68" s="50"/>
+      <c r="O68" s="50"/>
       <c r="FS68"/>
       <c r="FT68"/>
       <c r="FU68"/>
@@ -64773,40 +64789,40 @@
       <c r="AMJ68"/>
     </row>
     <row r="69" spans="1:1254" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="31" t="s">
-        <v>117</v>
+      <c r="A69" s="27" t="s">
+        <v>115</v>
       </c>
-      <c r="B69" s="15">
+      <c r="B69" s="14">
         <v>20.25</v>
       </c>
-      <c r="C69" s="32">
+      <c r="C69" s="28">
         <v>1</v>
       </c>
-      <c r="D69" s="17">
+      <c r="D69" s="16">
         <f t="shared" ref="D69:D70" si="6">B69*C69</f>
         <v>20.25</v>
       </c>
-      <c r="E69" s="33" t="s">
-        <v>20</v>
+      <c r="E69" s="29" t="s">
+        <v>19</v>
       </c>
-      <c r="F69" s="34" t="s">
-        <v>118</v>
+      <c r="F69" s="30" t="s">
+        <v>116</v>
       </c>
-      <c r="G69" s="32" t="s">
-        <v>86</v>
+      <c r="G69" s="28" t="s">
+        <v>84</v>
       </c>
-      <c r="H69" s="26" t="s">
-        <v>144</v>
+      <c r="H69" s="55" t="s">
+        <v>142</v>
       </c>
-      <c r="I69" s="39"/>
-      <c r="J69" s="58" t="s">
-        <v>121</v>
+      <c r="I69" s="34"/>
+      <c r="J69" s="50" t="s">
+        <v>119</v>
       </c>
-      <c r="K69" s="58"/>
-      <c r="L69" s="58"/>
-      <c r="M69" s="58"/>
-      <c r="N69" s="58"/>
-      <c r="O69" s="58"/>
+      <c r="K69" s="50"/>
+      <c r="L69" s="50"/>
+      <c r="M69" s="50"/>
+      <c r="N69" s="50"/>
+      <c r="O69" s="50"/>
       <c r="FS69"/>
       <c r="FT69"/>
       <c r="FU69"/>
@@ -65659,40 +65675,40 @@
       <c r="AMJ69"/>
     </row>
     <row r="70" spans="1:1254" s="4" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="31" t="s">
-        <v>119</v>
+      <c r="A70" s="27" t="s">
+        <v>117</v>
       </c>
-      <c r="B70" s="15">
+      <c r="B70" s="14">
         <v>2.63</v>
       </c>
-      <c r="C70" s="32">
+      <c r="C70" s="28">
         <v>3</v>
       </c>
-      <c r="D70" s="17">
+      <c r="D70" s="16">
         <f t="shared" si="6"/>
         <v>7.89</v>
       </c>
-      <c r="E70" s="33" t="s">
-        <v>20</v>
+      <c r="E70" s="29" t="s">
+        <v>19</v>
       </c>
-      <c r="F70" s="34" t="s">
+      <c r="F70" s="30" t="s">
+        <v>118</v>
+      </c>
+      <c r="G70" s="28" t="s">
+        <v>84</v>
+      </c>
+      <c r="H70" s="55" t="s">
+        <v>142</v>
+      </c>
+      <c r="I70" s="34"/>
+      <c r="J70" s="50" t="s">
         <v>120</v>
       </c>
-      <c r="G70" s="32" t="s">
-        <v>86</v>
-      </c>
-      <c r="H70" s="26" t="s">
-        <v>144</v>
-      </c>
-      <c r="I70" s="39"/>
-      <c r="J70" s="58" t="s">
-        <v>122</v>
-      </c>
-      <c r="K70" s="58"/>
-      <c r="L70" s="58"/>
-      <c r="M70" s="58"/>
-      <c r="N70" s="58"/>
-      <c r="O70" s="58"/>
+      <c r="K70" s="50"/>
+      <c r="L70" s="50"/>
+      <c r="M70" s="50"/>
+      <c r="N70" s="50"/>
+      <c r="O70" s="50"/>
       <c r="P70"/>
       <c r="Q70"/>
       <c r="R70"/>
@@ -66934,12 +66950,12 @@
       <c r="AVF70"/>
     </row>
     <row r="71" spans="1:1254" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="53" t="s">
-        <v>132</v>
+      <c r="A71" s="58" t="s">
+        <v>130</v>
       </c>
-      <c r="B71" s="54"/>
-      <c r="C71" s="55"/>
-      <c r="D71" s="13">
+      <c r="B71" s="59"/>
+      <c r="C71" s="60"/>
+      <c r="D71" s="61">
         <f>SUM(D3:D5,D7:D21,D23:D28,D30:D35,D37:D42,D46:D63,D68:D70)</f>
         <v>2120.8760000000002</v>
       </c>
@@ -69511,19 +69527,48 @@
     </row>
   </sheetData>
   <mergeCells count="71">
-    <mergeCell ref="J30:O30"/>
-    <mergeCell ref="J31:O31"/>
-    <mergeCell ref="A29:O29"/>
-    <mergeCell ref="J68:O68"/>
-    <mergeCell ref="A36:O36"/>
-    <mergeCell ref="J62:O62"/>
-    <mergeCell ref="J57:O57"/>
-    <mergeCell ref="J56:O56"/>
-    <mergeCell ref="J55:O55"/>
-    <mergeCell ref="J54:O54"/>
-    <mergeCell ref="J53:O53"/>
-    <mergeCell ref="J46:O46"/>
-    <mergeCell ref="J48:O48"/>
+    <mergeCell ref="A71:C71"/>
+    <mergeCell ref="J37:N37"/>
+    <mergeCell ref="J41:N41"/>
+    <mergeCell ref="J40:N40"/>
+    <mergeCell ref="J39:N39"/>
+    <mergeCell ref="J38:N38"/>
+    <mergeCell ref="J44:N44"/>
+    <mergeCell ref="J43:N43"/>
+    <mergeCell ref="J42:N42"/>
+    <mergeCell ref="J13:O13"/>
+    <mergeCell ref="J14:O14"/>
+    <mergeCell ref="J70:O70"/>
+    <mergeCell ref="J69:O69"/>
+    <mergeCell ref="J20:O20"/>
+    <mergeCell ref="J28:O28"/>
+    <mergeCell ref="J65:O65"/>
+    <mergeCell ref="J66:O66"/>
+    <mergeCell ref="A45:O45"/>
+    <mergeCell ref="A67:O67"/>
+    <mergeCell ref="A64:O64"/>
+    <mergeCell ref="J52:O52"/>
+    <mergeCell ref="J51:O51"/>
+    <mergeCell ref="J50:O50"/>
+    <mergeCell ref="J47:O47"/>
+    <mergeCell ref="J15:O15"/>
+    <mergeCell ref="J8:O8"/>
+    <mergeCell ref="J9:O9"/>
+    <mergeCell ref="J10:O10"/>
+    <mergeCell ref="J11:O11"/>
+    <mergeCell ref="J12:O12"/>
+    <mergeCell ref="J1:O1"/>
+    <mergeCell ref="J3:O3"/>
+    <mergeCell ref="J4:O4"/>
+    <mergeCell ref="J5:O5"/>
+    <mergeCell ref="J7:O7"/>
+    <mergeCell ref="A6:O6"/>
+    <mergeCell ref="A2:O2"/>
+    <mergeCell ref="J16:O16"/>
+    <mergeCell ref="J17:O17"/>
+    <mergeCell ref="J18:O18"/>
+    <mergeCell ref="J19:O19"/>
+    <mergeCell ref="J23:O23"/>
     <mergeCell ref="J24:O24"/>
     <mergeCell ref="J25:O25"/>
     <mergeCell ref="A22:O22"/>
@@ -69540,48 +69585,19 @@
     <mergeCell ref="J60:O60"/>
     <mergeCell ref="J26:O26"/>
     <mergeCell ref="J27:O27"/>
-    <mergeCell ref="J16:O16"/>
-    <mergeCell ref="J17:O17"/>
-    <mergeCell ref="J18:O18"/>
-    <mergeCell ref="J19:O19"/>
-    <mergeCell ref="J23:O23"/>
-    <mergeCell ref="J1:O1"/>
-    <mergeCell ref="J3:O3"/>
-    <mergeCell ref="J4:O4"/>
-    <mergeCell ref="J5:O5"/>
-    <mergeCell ref="J7:O7"/>
-    <mergeCell ref="A6:O6"/>
-    <mergeCell ref="A2:O2"/>
-    <mergeCell ref="J8:O8"/>
-    <mergeCell ref="J9:O9"/>
-    <mergeCell ref="J10:O10"/>
-    <mergeCell ref="J11:O11"/>
-    <mergeCell ref="J12:O12"/>
-    <mergeCell ref="J13:O13"/>
-    <mergeCell ref="J14:O14"/>
-    <mergeCell ref="J70:O70"/>
-    <mergeCell ref="J69:O69"/>
-    <mergeCell ref="J20:O20"/>
-    <mergeCell ref="J28:O28"/>
-    <mergeCell ref="J65:O65"/>
-    <mergeCell ref="J66:O66"/>
-    <mergeCell ref="A45:O45"/>
-    <mergeCell ref="A67:O67"/>
-    <mergeCell ref="A64:O64"/>
-    <mergeCell ref="J52:O52"/>
-    <mergeCell ref="J51:O51"/>
-    <mergeCell ref="J50:O50"/>
-    <mergeCell ref="J47:O47"/>
-    <mergeCell ref="J15:O15"/>
-    <mergeCell ref="A71:C71"/>
-    <mergeCell ref="J37:N37"/>
-    <mergeCell ref="J41:N41"/>
-    <mergeCell ref="J40:N40"/>
-    <mergeCell ref="J39:N39"/>
-    <mergeCell ref="J38:N38"/>
-    <mergeCell ref="J44:N44"/>
-    <mergeCell ref="J43:N43"/>
-    <mergeCell ref="J42:N42"/>
+    <mergeCell ref="J30:O30"/>
+    <mergeCell ref="J31:O31"/>
+    <mergeCell ref="A29:O29"/>
+    <mergeCell ref="J68:O68"/>
+    <mergeCell ref="A36:O36"/>
+    <mergeCell ref="J62:O62"/>
+    <mergeCell ref="J57:O57"/>
+    <mergeCell ref="J56:O56"/>
+    <mergeCell ref="J55:O55"/>
+    <mergeCell ref="J54:O54"/>
+    <mergeCell ref="J53:O53"/>
+    <mergeCell ref="J46:O46"/>
+    <mergeCell ref="J48:O48"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="H7" r:id="rId1" location="90967A160" tooltip="LINK"/>

</xml_diff>

<commit_message>
Modified component check list and EFS BOM
</commit_message>
<xml_diff>
--- a/Purchasing/EFS_BOM.xlsx
+++ b/Purchasing/EFS_BOM.xlsx
@@ -222,9 +222,6 @@
   </si>
   <si>
     <t>1SPA</t>
-  </si>
-  <si>
-    <t>Shaft</t>
   </si>
   <si>
     <t>1SFTA</t>
@@ -492,6 +489,9 @@
   </si>
   <si>
     <t>Used as the initial spec seal</t>
+  </si>
+  <si>
+    <t>Impeller Shaft</t>
   </si>
 </sst>
 </file>
@@ -880,24 +880,6 @@
     <xf numFmtId="0" fontId="13" fillId="6" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -910,6 +892,12 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="7" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -919,17 +907,29 @@
     <xf numFmtId="0" fontId="8" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="7" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1285,7 +1285,7 @@
   <dimension ref="A1:AVF73"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13:O13"/>
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1307,7 +1307,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1254" s="2" customFormat="1" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="53" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
@@ -1329,19 +1329,19 @@
         <v>6</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
-      <c r="J1" s="51" t="s">
+      <c r="J1" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="51"/>
-      <c r="L1" s="51"/>
-      <c r="M1" s="51"/>
-      <c r="N1" s="51"/>
-      <c r="O1" s="51"/>
+      <c r="K1" s="62"/>
+      <c r="L1" s="62"/>
+      <c r="M1" s="62"/>
+      <c r="N1" s="62"/>
+      <c r="O1" s="62"/>
       <c r="P1"/>
       <c r="Q1"/>
       <c r="R1"/>
@@ -2583,23 +2583,23 @@
       <c r="AVF1"/>
     </row>
     <row r="2" spans="1:1254" s="3" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="62" t="s">
+      <c r="A2" s="61" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="62"/>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="62"/>
-      <c r="I2" s="62"/>
-      <c r="J2" s="62"/>
-      <c r="K2" s="62"/>
-      <c r="L2" s="62"/>
-      <c r="M2" s="62"/>
-      <c r="N2" s="62"/>
-      <c r="O2" s="62"/>
+      <c r="B2" s="61"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="61"/>
+      <c r="J2" s="61"/>
+      <c r="K2" s="61"/>
+      <c r="L2" s="61"/>
+      <c r="M2" s="61"/>
+      <c r="N2" s="61"/>
+      <c r="O2" s="61"/>
       <c r="P2"/>
       <c r="Q2"/>
       <c r="R2"/>
@@ -3863,16 +3863,16 @@
       <c r="G3" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="54"/>
+      <c r="H3" s="48"/>
       <c r="I3" s="21"/>
-      <c r="J3" s="48" t="s">
+      <c r="J3" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="K3" s="48"/>
-      <c r="L3" s="48"/>
-      <c r="M3" s="48"/>
-      <c r="N3" s="48"/>
-      <c r="O3" s="48"/>
+      <c r="K3" s="58"/>
+      <c r="L3" s="58"/>
+      <c r="M3" s="58"/>
+      <c r="N3" s="58"/>
+      <c r="O3" s="58"/>
       <c r="FS3"/>
       <c r="FT3"/>
       <c r="FU3"/>
@@ -4747,16 +4747,16 @@
       <c r="G4" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="54"/>
+      <c r="H4" s="48"/>
       <c r="I4" s="21"/>
-      <c r="J4" s="48" t="s">
+      <c r="J4" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="K4" s="48"/>
-      <c r="L4" s="48"/>
-      <c r="M4" s="48"/>
-      <c r="N4" s="48"/>
-      <c r="O4" s="48"/>
+      <c r="K4" s="58"/>
+      <c r="L4" s="58"/>
+      <c r="M4" s="58"/>
+      <c r="N4" s="58"/>
+      <c r="O4" s="58"/>
       <c r="FS4"/>
       <c r="FT4"/>
       <c r="FU4"/>
@@ -5631,16 +5631,16 @@
       <c r="G5" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="54"/>
+      <c r="H5" s="48"/>
       <c r="I5" s="21"/>
-      <c r="J5" s="48" t="s">
+      <c r="J5" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="K5" s="48"/>
-      <c r="L5" s="48"/>
-      <c r="M5" s="48"/>
-      <c r="N5" s="48"/>
-      <c r="O5" s="48"/>
+      <c r="K5" s="58"/>
+      <c r="L5" s="58"/>
+      <c r="M5" s="58"/>
+      <c r="N5" s="58"/>
+      <c r="O5" s="58"/>
       <c r="FS5"/>
       <c r="FT5"/>
       <c r="FU5"/>
@@ -6493,23 +6493,23 @@
       <c r="AMJ5"/>
     </row>
     <row r="6" spans="1:1254" s="4" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="62" t="s">
-        <v>154</v>
+      <c r="A6" s="61" t="s">
+        <v>153</v>
       </c>
-      <c r="B6" s="62"/>
-      <c r="C6" s="62"/>
-      <c r="D6" s="62"/>
-      <c r="E6" s="62"/>
-      <c r="F6" s="62"/>
-      <c r="G6" s="62"/>
-      <c r="H6" s="62"/>
-      <c r="I6" s="62"/>
-      <c r="J6" s="62"/>
-      <c r="K6" s="62"/>
-      <c r="L6" s="62"/>
-      <c r="M6" s="62"/>
-      <c r="N6" s="62"/>
-      <c r="O6" s="62"/>
+      <c r="B6" s="61"/>
+      <c r="C6" s="61"/>
+      <c r="D6" s="61"/>
+      <c r="E6" s="61"/>
+      <c r="F6" s="61"/>
+      <c r="G6" s="61"/>
+      <c r="H6" s="61"/>
+      <c r="I6" s="61"/>
+      <c r="J6" s="61"/>
+      <c r="K6" s="61"/>
+      <c r="L6" s="61"/>
+      <c r="M6" s="61"/>
+      <c r="N6" s="61"/>
+      <c r="O6" s="61"/>
       <c r="P6"/>
       <c r="Q6"/>
       <c r="R6"/>
@@ -7773,18 +7773,18 @@
       <c r="G7" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="55" t="s">
-        <v>142</v>
+      <c r="H7" s="49" t="s">
+        <v>141</v>
       </c>
       <c r="I7" s="24"/>
-      <c r="J7" s="48" t="s">
+      <c r="J7" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="K7" s="48"/>
-      <c r="L7" s="48"/>
-      <c r="M7" s="48"/>
-      <c r="N7" s="48"/>
-      <c r="O7" s="48"/>
+      <c r="K7" s="58"/>
+      <c r="L7" s="58"/>
+      <c r="M7" s="58"/>
+      <c r="N7" s="58"/>
+      <c r="O7" s="58"/>
       <c r="FS7"/>
       <c r="FT7"/>
       <c r="FU7"/>
@@ -8659,14 +8659,14 @@
       <c r="G8" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H8" s="56"/>
+      <c r="H8" s="50"/>
       <c r="I8" s="24"/>
-      <c r="J8" s="48"/>
-      <c r="K8" s="48"/>
-      <c r="L8" s="48"/>
-      <c r="M8" s="48"/>
-      <c r="N8" s="48"/>
-      <c r="O8" s="48"/>
+      <c r="J8" s="58"/>
+      <c r="K8" s="58"/>
+      <c r="L8" s="58"/>
+      <c r="M8" s="58"/>
+      <c r="N8" s="58"/>
+      <c r="O8" s="58"/>
       <c r="FS8"/>
       <c r="FT8"/>
       <c r="FU8"/>
@@ -9541,14 +9541,14 @@
       <c r="G9" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H9" s="56"/>
+      <c r="H9" s="50"/>
       <c r="I9" s="24"/>
-      <c r="J9" s="48"/>
-      <c r="K9" s="48"/>
-      <c r="L9" s="48"/>
-      <c r="M9" s="48"/>
-      <c r="N9" s="48"/>
-      <c r="O9" s="48"/>
+      <c r="J9" s="58"/>
+      <c r="K9" s="58"/>
+      <c r="L9" s="58"/>
+      <c r="M9" s="58"/>
+      <c r="N9" s="58"/>
+      <c r="O9" s="58"/>
       <c r="FS9"/>
       <c r="FT9"/>
       <c r="FU9"/>
@@ -10423,16 +10423,16 @@
       <c r="G10" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H10" s="55" t="s">
-        <v>142</v>
+      <c r="H10" s="49" t="s">
+        <v>141</v>
       </c>
       <c r="I10" s="24"/>
-      <c r="J10" s="48"/>
-      <c r="K10" s="48"/>
-      <c r="L10" s="48"/>
-      <c r="M10" s="48"/>
-      <c r="N10" s="48"/>
-      <c r="O10" s="48"/>
+      <c r="J10" s="58"/>
+      <c r="K10" s="58"/>
+      <c r="L10" s="58"/>
+      <c r="M10" s="58"/>
+      <c r="N10" s="58"/>
+      <c r="O10" s="58"/>
       <c r="FS10"/>
       <c r="FT10"/>
       <c r="FU10"/>
@@ -11307,18 +11307,18 @@
       <c r="G11" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H11" s="55" t="s">
-        <v>142</v>
+      <c r="H11" s="49" t="s">
+        <v>141</v>
       </c>
       <c r="I11" s="24"/>
-      <c r="J11" s="48" t="s">
+      <c r="J11" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="K11" s="48"/>
-      <c r="L11" s="48"/>
-      <c r="M11" s="48"/>
-      <c r="N11" s="48"/>
-      <c r="O11" s="48"/>
+      <c r="K11" s="58"/>
+      <c r="L11" s="58"/>
+      <c r="M11" s="58"/>
+      <c r="N11" s="58"/>
+      <c r="O11" s="58"/>
       <c r="FS11"/>
       <c r="FT11"/>
       <c r="FU11"/>
@@ -12172,7 +12172,7 @@
     </row>
     <row r="12" spans="1:1254" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="25" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B12" s="16">
         <v>8.11</v>
@@ -12193,16 +12193,16 @@
       <c r="G12" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H12" s="56"/>
+      <c r="H12" s="50"/>
       <c r="I12" s="24"/>
-      <c r="J12" s="48" t="s">
-        <v>150</v>
+      <c r="J12" s="58" t="s">
+        <v>149</v>
       </c>
-      <c r="K12" s="48"/>
-      <c r="L12" s="48"/>
-      <c r="M12" s="48"/>
-      <c r="N12" s="48"/>
-      <c r="O12" s="48"/>
+      <c r="K12" s="58"/>
+      <c r="L12" s="58"/>
+      <c r="M12" s="58"/>
+      <c r="N12" s="58"/>
+      <c r="O12" s="58"/>
       <c r="FS12"/>
       <c r="FT12"/>
       <c r="FU12"/>
@@ -13077,16 +13077,16 @@
       <c r="G13" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H13" s="56"/>
+      <c r="H13" s="50"/>
       <c r="I13" s="24"/>
-      <c r="J13" s="48" t="s">
+      <c r="J13" s="58" t="s">
         <v>34</v>
       </c>
-      <c r="K13" s="48"/>
-      <c r="L13" s="48"/>
-      <c r="M13" s="48"/>
-      <c r="N13" s="48"/>
-      <c r="O13" s="48"/>
+      <c r="K13" s="58"/>
+      <c r="L13" s="58"/>
+      <c r="M13" s="58"/>
+      <c r="N13" s="58"/>
+      <c r="O13" s="58"/>
       <c r="FS13"/>
       <c r="FT13"/>
       <c r="FU13"/>
@@ -13940,7 +13940,7 @@
     </row>
     <row r="14" spans="1:1254" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="25" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B14" s="16">
         <v>6.01</v>
@@ -13961,16 +13961,16 @@
       <c r="G14" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H14" s="56"/>
+      <c r="H14" s="50"/>
       <c r="I14" s="24"/>
-      <c r="J14" s="48" t="s">
-        <v>153</v>
+      <c r="J14" s="58" t="s">
+        <v>152</v>
       </c>
-      <c r="K14" s="48"/>
-      <c r="L14" s="48"/>
-      <c r="M14" s="48"/>
-      <c r="N14" s="48"/>
-      <c r="O14" s="48"/>
+      <c r="K14" s="58"/>
+      <c r="L14" s="58"/>
+      <c r="M14" s="58"/>
+      <c r="N14" s="58"/>
+      <c r="O14" s="58"/>
       <c r="FS14"/>
       <c r="FT14"/>
       <c r="FU14"/>
@@ -14845,16 +14845,16 @@
       <c r="G15" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H15" s="56"/>
+      <c r="H15" s="50"/>
       <c r="I15" s="24"/>
-      <c r="J15" s="48" t="s">
+      <c r="J15" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="K15" s="48"/>
-      <c r="L15" s="48"/>
-      <c r="M15" s="48"/>
-      <c r="N15" s="48"/>
-      <c r="O15" s="48"/>
+      <c r="K15" s="58"/>
+      <c r="L15" s="58"/>
+      <c r="M15" s="58"/>
+      <c r="N15" s="58"/>
+      <c r="O15" s="58"/>
       <c r="FS15"/>
       <c r="FT15"/>
       <c r="FU15"/>
@@ -15729,14 +15729,14 @@
       <c r="G16" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H16" s="56"/>
+      <c r="H16" s="50"/>
       <c r="I16" s="24"/>
-      <c r="J16" s="48"/>
-      <c r="K16" s="48"/>
-      <c r="L16" s="48"/>
-      <c r="M16" s="48"/>
-      <c r="N16" s="48"/>
-      <c r="O16" s="48"/>
+      <c r="J16" s="58"/>
+      <c r="K16" s="58"/>
+      <c r="L16" s="58"/>
+      <c r="M16" s="58"/>
+      <c r="N16" s="58"/>
+      <c r="O16" s="58"/>
       <c r="FS16"/>
       <c r="FT16"/>
       <c r="FU16"/>
@@ -16590,7 +16590,7 @@
     </row>
     <row r="17" spans="1:1254" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="25" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B17" s="16">
         <v>20.7</v>
@@ -16611,16 +16611,16 @@
       <c r="G17" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H17" s="56"/>
+      <c r="H17" s="50"/>
       <c r="I17" s="24"/>
-      <c r="J17" s="48" t="s">
-        <v>145</v>
+      <c r="J17" s="58" t="s">
+        <v>144</v>
       </c>
-      <c r="K17" s="48"/>
-      <c r="L17" s="48"/>
-      <c r="M17" s="48"/>
-      <c r="N17" s="48"/>
-      <c r="O17" s="48"/>
+      <c r="K17" s="58"/>
+      <c r="L17" s="58"/>
+      <c r="M17" s="58"/>
+      <c r="N17" s="58"/>
+      <c r="O17" s="58"/>
       <c r="FS17"/>
       <c r="FT17"/>
       <c r="FU17"/>
@@ -17474,7 +17474,7 @@
     </row>
     <row r="18" spans="1:1254" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="25" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B18" s="16">
         <v>5.68</v>
@@ -17495,14 +17495,14 @@
       <c r="G18" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H18" s="56"/>
+      <c r="H18" s="50"/>
       <c r="I18" s="24"/>
-      <c r="J18" s="48"/>
-      <c r="K18" s="48"/>
-      <c r="L18" s="48"/>
-      <c r="M18" s="48"/>
-      <c r="N18" s="48"/>
-      <c r="O18" s="48"/>
+      <c r="J18" s="58"/>
+      <c r="K18" s="58"/>
+      <c r="L18" s="58"/>
+      <c r="M18" s="58"/>
+      <c r="N18" s="58"/>
+      <c r="O18" s="58"/>
       <c r="FS18"/>
       <c r="FT18"/>
       <c r="FU18"/>
@@ -18356,7 +18356,7 @@
     </row>
     <row r="19" spans="1:1254" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="25" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B19" s="16">
         <v>2.6</v>
@@ -18377,18 +18377,18 @@
       <c r="G19" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H19" s="55" t="s">
-        <v>142</v>
+      <c r="H19" s="49" t="s">
+        <v>141</v>
       </c>
       <c r="I19" s="24"/>
-      <c r="J19" s="48" t="s">
-        <v>148</v>
+      <c r="J19" s="58" t="s">
+        <v>147</v>
       </c>
-      <c r="K19" s="48"/>
-      <c r="L19" s="48"/>
-      <c r="M19" s="48"/>
-      <c r="N19" s="48"/>
-      <c r="O19" s="48"/>
+      <c r="K19" s="58"/>
+      <c r="L19" s="58"/>
+      <c r="M19" s="58"/>
+      <c r="N19" s="58"/>
+      <c r="O19" s="58"/>
       <c r="FS19"/>
       <c r="FT19"/>
       <c r="FU19"/>
@@ -19242,7 +19242,7 @@
     </row>
     <row r="20" spans="1:1254" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="27" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B20" s="14">
         <v>23.82</v>
@@ -19258,23 +19258,23 @@
         <v>19</v>
       </c>
       <c r="F20" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="G20" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="H20" s="49" t="s">
+        <v>141</v>
+      </c>
+      <c r="I20" s="31"/>
+      <c r="J20" s="58" t="s">
         <v>122</v>
       </c>
-      <c r="G20" s="28" t="s">
-        <v>84</v>
-      </c>
-      <c r="H20" s="55" t="s">
-        <v>142</v>
-      </c>
-      <c r="I20" s="31"/>
-      <c r="J20" s="48" t="s">
-        <v>123</v>
-      </c>
-      <c r="K20" s="48"/>
-      <c r="L20" s="48"/>
-      <c r="M20" s="48"/>
-      <c r="N20" s="48"/>
-      <c r="O20" s="48"/>
+      <c r="K20" s="58"/>
+      <c r="L20" s="58"/>
+      <c r="M20" s="58"/>
+      <c r="N20" s="58"/>
+      <c r="O20" s="58"/>
       <c r="FS20"/>
       <c r="FT20"/>
       <c r="FU20"/>
@@ -20128,7 +20128,7 @@
     </row>
     <row r="21" spans="1:1254" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B21" s="16">
         <v>25.93</v>
@@ -20144,23 +20144,23 @@
         <v>19</v>
       </c>
       <c r="F21" s="23" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G21" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H21" s="55" t="s">
-        <v>142</v>
+      <c r="H21" s="49" t="s">
+        <v>141</v>
       </c>
       <c r="I21" s="32"/>
-      <c r="J21" s="48" t="s">
-        <v>155</v>
+      <c r="J21" s="58" t="s">
+        <v>154</v>
       </c>
-      <c r="K21" s="48"/>
-      <c r="L21" s="48"/>
-      <c r="M21" s="48"/>
-      <c r="N21" s="48"/>
-      <c r="O21" s="48"/>
+      <c r="K21" s="58"/>
+      <c r="L21" s="58"/>
+      <c r="M21" s="58"/>
+      <c r="N21" s="58"/>
+      <c r="O21" s="58"/>
       <c r="FS21"/>
       <c r="FT21"/>
       <c r="FU21"/>
@@ -21013,23 +21013,23 @@
       <c r="AMJ21"/>
     </row>
     <row r="22" spans="1:1254" s="4" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="62" t="s">
+      <c r="A22" s="61" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="62"/>
-      <c r="C22" s="62"/>
-      <c r="D22" s="62"/>
-      <c r="E22" s="62"/>
-      <c r="F22" s="62"/>
-      <c r="G22" s="62"/>
-      <c r="H22" s="62"/>
-      <c r="I22" s="62"/>
-      <c r="J22" s="62"/>
-      <c r="K22" s="62"/>
-      <c r="L22" s="62"/>
-      <c r="M22" s="62"/>
-      <c r="N22" s="62"/>
-      <c r="O22" s="62"/>
+      <c r="B22" s="61"/>
+      <c r="C22" s="61"/>
+      <c r="D22" s="61"/>
+      <c r="E22" s="61"/>
+      <c r="F22" s="61"/>
+      <c r="G22" s="61"/>
+      <c r="H22" s="61"/>
+      <c r="I22" s="61"/>
+      <c r="J22" s="61"/>
+      <c r="K22" s="61"/>
+      <c r="L22" s="61"/>
+      <c r="M22" s="61"/>
+      <c r="N22" s="61"/>
+      <c r="O22" s="61"/>
       <c r="P22"/>
       <c r="Q22"/>
       <c r="R22"/>
@@ -22293,16 +22293,16 @@
       <c r="G23" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H23" s="55" t="s">
-        <v>142</v>
+      <c r="H23" s="49" t="s">
+        <v>141</v>
       </c>
       <c r="I23" s="33"/>
-      <c r="J23" s="48"/>
-      <c r="K23" s="48"/>
-      <c r="L23" s="48"/>
-      <c r="M23" s="48"/>
-      <c r="N23" s="48"/>
-      <c r="O23" s="48"/>
+      <c r="J23" s="58"/>
+      <c r="K23" s="58"/>
+      <c r="L23" s="58"/>
+      <c r="M23" s="58"/>
+      <c r="N23" s="58"/>
+      <c r="O23" s="58"/>
       <c r="FS23"/>
       <c r="FT23"/>
       <c r="FU23"/>
@@ -23156,7 +23156,7 @@
     </row>
     <row r="24" spans="1:1254" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B24" s="16">
         <v>247.07</v>
@@ -23177,16 +23177,16 @@
       <c r="G24" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H24" s="55" t="s">
-        <v>142</v>
+      <c r="H24" s="49" t="s">
+        <v>141</v>
       </c>
       <c r="I24" s="33"/>
-      <c r="J24" s="48"/>
-      <c r="K24" s="48"/>
-      <c r="L24" s="48"/>
-      <c r="M24" s="48"/>
-      <c r="N24" s="48"/>
-      <c r="O24" s="48"/>
+      <c r="J24" s="58"/>
+      <c r="K24" s="58"/>
+      <c r="L24" s="58"/>
+      <c r="M24" s="58"/>
+      <c r="N24" s="58"/>
+      <c r="O24" s="58"/>
       <c r="FS24"/>
       <c r="FT24"/>
       <c r="FU24"/>
@@ -24061,16 +24061,16 @@
       <c r="G25" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H25" s="55" t="s">
-        <v>142</v>
+      <c r="H25" s="49" t="s">
+        <v>141</v>
       </c>
       <c r="I25" s="33"/>
-      <c r="J25" s="48"/>
-      <c r="K25" s="48"/>
-      <c r="L25" s="48"/>
-      <c r="M25" s="48"/>
-      <c r="N25" s="48"/>
-      <c r="O25" s="48"/>
+      <c r="J25" s="58"/>
+      <c r="K25" s="58"/>
+      <c r="L25" s="58"/>
+      <c r="M25" s="58"/>
+      <c r="N25" s="58"/>
+      <c r="O25" s="58"/>
       <c r="FS25"/>
       <c r="FT25"/>
       <c r="FU25"/>
@@ -24945,16 +24945,16 @@
       <c r="G26" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H26" s="55" t="s">
-        <v>142</v>
+      <c r="H26" s="49" t="s">
+        <v>141</v>
       </c>
       <c r="I26" s="33"/>
-      <c r="J26" s="48"/>
-      <c r="K26" s="48"/>
-      <c r="L26" s="48"/>
-      <c r="M26" s="48"/>
-      <c r="N26" s="48"/>
-      <c r="O26" s="48"/>
+      <c r="J26" s="58"/>
+      <c r="K26" s="58"/>
+      <c r="L26" s="58"/>
+      <c r="M26" s="58"/>
+      <c r="N26" s="58"/>
+      <c r="O26" s="58"/>
       <c r="FS26"/>
       <c r="FT26"/>
       <c r="FU26"/>
@@ -25829,16 +25829,16 @@
       <c r="G27" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H27" s="55" t="s">
-        <v>142</v>
+      <c r="H27" s="49" t="s">
+        <v>141</v>
       </c>
       <c r="I27" s="33"/>
-      <c r="J27" s="48"/>
-      <c r="K27" s="48"/>
-      <c r="L27" s="48"/>
-      <c r="M27" s="48"/>
-      <c r="N27" s="48"/>
-      <c r="O27" s="48"/>
+      <c r="J27" s="58"/>
+      <c r="K27" s="58"/>
+      <c r="L27" s="58"/>
+      <c r="M27" s="58"/>
+      <c r="N27" s="58"/>
+      <c r="O27" s="58"/>
       <c r="FS27"/>
       <c r="FT27"/>
       <c r="FU27"/>
@@ -26692,7 +26692,7 @@
     </row>
     <row r="28" spans="1:1254" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="27" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B28" s="14">
         <v>153.85</v>
@@ -26705,24 +26705,24 @@
         <v>153.85</v>
       </c>
       <c r="E28" s="29" t="s">
+        <v>124</v>
+      </c>
+      <c r="F28" s="30" t="s">
         <v>125</v>
       </c>
-      <c r="F28" s="30" t="s">
-        <v>126</v>
+      <c r="G28" s="28" t="s">
+        <v>83</v>
       </c>
-      <c r="G28" s="28" t="s">
-        <v>84</v>
-      </c>
-      <c r="H28" s="57" t="s">
-        <v>142</v>
+      <c r="H28" s="51" t="s">
+        <v>141</v>
       </c>
       <c r="I28" s="34"/>
-      <c r="J28" s="48"/>
-      <c r="K28" s="48"/>
-      <c r="L28" s="48"/>
-      <c r="M28" s="48"/>
-      <c r="N28" s="48"/>
-      <c r="O28" s="48"/>
+      <c r="J28" s="58"/>
+      <c r="K28" s="58"/>
+      <c r="L28" s="58"/>
+      <c r="M28" s="58"/>
+      <c r="N28" s="58"/>
+      <c r="O28" s="58"/>
       <c r="FS28"/>
       <c r="FT28"/>
       <c r="FU28"/>
@@ -27575,23 +27575,23 @@
       <c r="AMJ28"/>
     </row>
     <row r="29" spans="1:1254" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="49" t="s">
+      <c r="A29" s="63" t="s">
         <v>54</v>
       </c>
-      <c r="B29" s="49"/>
-      <c r="C29" s="49"/>
-      <c r="D29" s="49"/>
-      <c r="E29" s="49"/>
-      <c r="F29" s="49"/>
-      <c r="G29" s="49"/>
-      <c r="H29" s="49"/>
-      <c r="I29" s="49"/>
-      <c r="J29" s="49"/>
-      <c r="K29" s="49"/>
-      <c r="L29" s="49"/>
-      <c r="M29" s="49"/>
-      <c r="N29" s="49"/>
-      <c r="O29" s="49"/>
+      <c r="B29" s="63"/>
+      <c r="C29" s="63"/>
+      <c r="D29" s="63"/>
+      <c r="E29" s="63"/>
+      <c r="F29" s="63"/>
+      <c r="G29" s="63"/>
+      <c r="H29" s="63"/>
+      <c r="I29" s="63"/>
+      <c r="J29" s="63"/>
+      <c r="K29" s="63"/>
+      <c r="L29" s="63"/>
+      <c r="M29" s="63"/>
+      <c r="N29" s="63"/>
+      <c r="O29" s="63"/>
       <c r="P29"/>
       <c r="Q29"/>
       <c r="R29"/>
@@ -28855,14 +28855,14 @@
       <c r="G30" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H30" s="54"/>
+      <c r="H30" s="48"/>
       <c r="I30" s="35"/>
-      <c r="J30" s="48"/>
-      <c r="K30" s="48"/>
-      <c r="L30" s="48"/>
-      <c r="M30" s="48"/>
-      <c r="N30" s="48"/>
-      <c r="O30" s="48"/>
+      <c r="J30" s="58"/>
+      <c r="K30" s="58"/>
+      <c r="L30" s="58"/>
+      <c r="M30" s="58"/>
+      <c r="N30" s="58"/>
+      <c r="O30" s="58"/>
       <c r="FS30"/>
       <c r="FT30"/>
       <c r="FU30"/>
@@ -29737,14 +29737,14 @@
       <c r="G31" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H31" s="54"/>
+      <c r="H31" s="48"/>
       <c r="I31" s="35"/>
-      <c r="J31" s="48"/>
-      <c r="K31" s="48"/>
-      <c r="L31" s="48"/>
-      <c r="M31" s="48"/>
-      <c r="N31" s="48"/>
-      <c r="O31" s="48"/>
+      <c r="J31" s="58"/>
+      <c r="K31" s="58"/>
+      <c r="L31" s="58"/>
+      <c r="M31" s="58"/>
+      <c r="N31" s="58"/>
+      <c r="O31" s="58"/>
       <c r="FS31"/>
       <c r="FT31"/>
       <c r="FU31"/>
@@ -30619,14 +30619,14 @@
       <c r="G32" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H32" s="54"/>
+      <c r="H32" s="48"/>
       <c r="I32" s="35"/>
-      <c r="J32" s="48"/>
-      <c r="K32" s="48"/>
-      <c r="L32" s="48"/>
-      <c r="M32" s="48"/>
-      <c r="N32" s="48"/>
-      <c r="O32" s="48"/>
+      <c r="J32" s="58"/>
+      <c r="K32" s="58"/>
+      <c r="L32" s="58"/>
+      <c r="M32" s="58"/>
+      <c r="N32" s="58"/>
+      <c r="O32" s="58"/>
       <c r="FS32"/>
       <c r="FT32"/>
       <c r="FU32"/>
@@ -31501,14 +31501,14 @@
       <c r="G33" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H33" s="54"/>
+      <c r="H33" s="48"/>
       <c r="I33" s="35"/>
-      <c r="J33" s="48"/>
-      <c r="K33" s="48"/>
-      <c r="L33" s="48"/>
-      <c r="M33" s="48"/>
-      <c r="N33" s="48"/>
-      <c r="O33" s="48"/>
+      <c r="J33" s="58"/>
+      <c r="K33" s="58"/>
+      <c r="L33" s="58"/>
+      <c r="M33" s="58"/>
+      <c r="N33" s="58"/>
+      <c r="O33" s="58"/>
       <c r="FS33"/>
       <c r="FT33"/>
       <c r="FU33"/>
@@ -32383,14 +32383,14 @@
       <c r="G34" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H34" s="54"/>
+      <c r="H34" s="48"/>
       <c r="I34" s="35"/>
-      <c r="J34" s="48"/>
-      <c r="K34" s="48"/>
-      <c r="L34" s="48"/>
-      <c r="M34" s="48"/>
-      <c r="N34" s="48"/>
-      <c r="O34" s="48"/>
+      <c r="J34" s="58"/>
+      <c r="K34" s="58"/>
+      <c r="L34" s="58"/>
+      <c r="M34" s="58"/>
+      <c r="N34" s="58"/>
+      <c r="O34" s="58"/>
       <c r="FS34"/>
       <c r="FT34"/>
       <c r="FU34"/>
@@ -33244,7 +33244,7 @@
     </row>
     <row r="35" spans="1:1254" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="10" t="s">
-        <v>66</v>
+        <v>155</v>
       </c>
       <c r="B35" s="15">
         <v>0</v>
@@ -33260,19 +33260,19 @@
         <v>56</v>
       </c>
       <c r="F35" s="20" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G35" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H35" s="54"/>
+      <c r="H35" s="48"/>
       <c r="I35" s="35"/>
-      <c r="J35" s="48"/>
-      <c r="K35" s="48"/>
-      <c r="L35" s="48"/>
-      <c r="M35" s="48"/>
-      <c r="N35" s="48"/>
-      <c r="O35" s="48"/>
+      <c r="J35" s="58"/>
+      <c r="K35" s="58"/>
+      <c r="L35" s="58"/>
+      <c r="M35" s="58"/>
+      <c r="N35" s="58"/>
+      <c r="O35" s="58"/>
       <c r="FS35"/>
       <c r="FT35"/>
       <c r="FU35"/>
@@ -34125,23 +34125,23 @@
       <c r="AMJ35"/>
     </row>
     <row r="36" spans="1:1254" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="63" t="s">
-        <v>77</v>
+      <c r="A36" s="64" t="s">
+        <v>76</v>
       </c>
-      <c r="B36" s="63"/>
-      <c r="C36" s="63"/>
-      <c r="D36" s="63"/>
-      <c r="E36" s="63"/>
-      <c r="F36" s="63"/>
-      <c r="G36" s="63"/>
-      <c r="H36" s="63"/>
-      <c r="I36" s="63"/>
-      <c r="J36" s="63"/>
-      <c r="K36" s="63"/>
-      <c r="L36" s="63"/>
-      <c r="M36" s="63"/>
-      <c r="N36" s="63"/>
-      <c r="O36" s="63"/>
+      <c r="B36" s="64"/>
+      <c r="C36" s="64"/>
+      <c r="D36" s="64"/>
+      <c r="E36" s="64"/>
+      <c r="F36" s="64"/>
+      <c r="G36" s="64"/>
+      <c r="H36" s="64"/>
+      <c r="I36" s="64"/>
+      <c r="J36" s="64"/>
+      <c r="K36" s="64"/>
+      <c r="L36" s="64"/>
+      <c r="M36" s="64"/>
+      <c r="N36" s="64"/>
+      <c r="O36" s="64"/>
       <c r="FS36"/>
       <c r="FT36"/>
       <c r="FU36"/>
@@ -34995,7 +34995,7 @@
     </row>
     <row r="37" spans="1:1254" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B37" s="15">
         <v>3.4495</v>
@@ -35008,23 +35008,23 @@
         <v>34.494999999999997</v>
       </c>
       <c r="E37" s="20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F37" s="20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G37" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H37" s="54"/>
+      <c r="H37" s="48"/>
       <c r="I37" s="21"/>
-      <c r="J37" s="53" t="s">
-        <v>134</v>
+      <c r="J37" s="57" t="s">
+        <v>133</v>
       </c>
-      <c r="K37" s="53"/>
-      <c r="L37" s="53"/>
-      <c r="M37" s="53"/>
-      <c r="N37" s="53"/>
+      <c r="K37" s="57"/>
+      <c r="L37" s="57"/>
+      <c r="M37" s="57"/>
+      <c r="N37" s="57"/>
       <c r="O37" s="10">
         <v>5</v>
       </c>
@@ -35881,7 +35881,7 @@
     </row>
     <row r="38" spans="1:1254" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B38" s="15">
         <v>3.45</v>
@@ -35894,23 +35894,23 @@
         <v>55.2</v>
       </c>
       <c r="E38" s="20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F38" s="20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G38" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H38" s="54"/>
+      <c r="H38" s="48"/>
       <c r="I38" s="21"/>
-      <c r="J38" s="53" t="s">
-        <v>134</v>
+      <c r="J38" s="57" t="s">
+        <v>133</v>
       </c>
-      <c r="K38" s="53"/>
-      <c r="L38" s="53"/>
-      <c r="M38" s="53"/>
-      <c r="N38" s="53"/>
+      <c r="K38" s="57"/>
+      <c r="L38" s="57"/>
+      <c r="M38" s="57"/>
+      <c r="N38" s="57"/>
       <c r="O38" s="10">
         <v>8</v>
       </c>
@@ -36767,7 +36767,7 @@
     </row>
     <row r="39" spans="1:1254" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B39" s="15">
         <v>3.4504999999999999</v>
@@ -36780,23 +36780,23 @@
         <v>27.603999999999999</v>
       </c>
       <c r="E39" s="20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F39" s="20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G39" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H39" s="54"/>
+      <c r="H39" s="48"/>
       <c r="I39" s="21"/>
-      <c r="J39" s="53" t="s">
-        <v>134</v>
+      <c r="J39" s="57" t="s">
+        <v>133</v>
       </c>
-      <c r="K39" s="53"/>
-      <c r="L39" s="53"/>
-      <c r="M39" s="53"/>
-      <c r="N39" s="53"/>
+      <c r="K39" s="57"/>
+      <c r="L39" s="57"/>
+      <c r="M39" s="57"/>
+      <c r="N39" s="57"/>
       <c r="O39" s="10">
         <v>4</v>
       </c>
@@ -37653,7 +37653,7 @@
     </row>
     <row r="40" spans="1:1254" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B40" s="15">
         <v>3.4510000000000001</v>
@@ -37666,23 +37666,23 @@
         <v>24.157</v>
       </c>
       <c r="E40" s="20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F40" s="20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G40" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H40" s="54"/>
+      <c r="H40" s="48"/>
       <c r="I40" s="21"/>
-      <c r="J40" s="53" t="s">
-        <v>134</v>
+      <c r="J40" s="57" t="s">
+        <v>133</v>
       </c>
-      <c r="K40" s="53"/>
-      <c r="L40" s="53"/>
-      <c r="M40" s="53"/>
-      <c r="N40" s="53"/>
+      <c r="K40" s="57"/>
+      <c r="L40" s="57"/>
+      <c r="M40" s="57"/>
+      <c r="N40" s="57"/>
       <c r="O40" s="10">
         <v>7</v>
       </c>
@@ -38539,7 +38539,7 @@
     </row>
     <row r="41" spans="1:1254" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B41" s="15">
         <v>5.3</v>
@@ -38552,23 +38552,23 @@
         <v>26.5</v>
       </c>
       <c r="E41" s="20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F41" s="20" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G41" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H41" s="54"/>
+      <c r="H41" s="48"/>
       <c r="I41" s="21"/>
-      <c r="J41" s="53" t="s">
-        <v>134</v>
+      <c r="J41" s="57" t="s">
+        <v>133</v>
       </c>
-      <c r="K41" s="53"/>
-      <c r="L41" s="53"/>
-      <c r="M41" s="53"/>
-      <c r="N41" s="53"/>
+      <c r="K41" s="57"/>
+      <c r="L41" s="57"/>
+      <c r="M41" s="57"/>
+      <c r="N41" s="57"/>
       <c r="O41" s="10">
         <v>5</v>
       </c>
@@ -39425,7 +39425,7 @@
     </row>
     <row r="42" spans="1:1254" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B42" s="15">
         <v>2.67</v>
@@ -39438,23 +39438,23 @@
         <v>8.01</v>
       </c>
       <c r="E42" s="20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F42" s="20" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G42" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H42" s="54"/>
+      <c r="H42" s="48"/>
       <c r="I42" s="21"/>
-      <c r="J42" s="53" t="s">
-        <v>134</v>
+      <c r="J42" s="57" t="s">
+        <v>133</v>
       </c>
-      <c r="K42" s="53"/>
-      <c r="L42" s="53"/>
-      <c r="M42" s="53"/>
-      <c r="N42" s="53"/>
+      <c r="K42" s="57"/>
+      <c r="L42" s="57"/>
+      <c r="M42" s="57"/>
+      <c r="N42" s="57"/>
       <c r="O42" s="10">
         <v>3</v>
       </c>
@@ -40311,7 +40311,7 @@
     </row>
     <row r="43" spans="1:1254" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B43" s="15">
         <v>1.65</v>
@@ -40324,23 +40324,23 @@
         <v>4.9499999999999993</v>
       </c>
       <c r="E43" s="20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F43" s="20" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G43" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H43" s="54"/>
+      <c r="H43" s="48"/>
       <c r="I43" s="21"/>
-      <c r="J43" s="53" t="s">
-        <v>134</v>
+      <c r="J43" s="57" t="s">
+        <v>133</v>
       </c>
-      <c r="K43" s="53"/>
-      <c r="L43" s="53"/>
-      <c r="M43" s="53"/>
-      <c r="N43" s="53"/>
+      <c r="K43" s="57"/>
+      <c r="L43" s="57"/>
+      <c r="M43" s="57"/>
+      <c r="N43" s="57"/>
       <c r="O43" s="10">
         <v>3</v>
       </c>
@@ -41197,7 +41197,7 @@
     </row>
     <row r="44" spans="1:1254" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B44" s="15">
         <v>2.1800000000000002</v>
@@ -41210,23 +41210,23 @@
         <v>13.080000000000002</v>
       </c>
       <c r="E44" s="20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F44" s="20" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G44" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H44" s="54"/>
+      <c r="H44" s="48"/>
       <c r="I44" s="21"/>
-      <c r="J44" s="53" t="s">
-        <v>134</v>
+      <c r="J44" s="57" t="s">
+        <v>133</v>
       </c>
-      <c r="K44" s="53"/>
-      <c r="L44" s="53"/>
-      <c r="M44" s="53"/>
-      <c r="N44" s="53"/>
+      <c r="K44" s="57"/>
+      <c r="L44" s="57"/>
+      <c r="M44" s="57"/>
+      <c r="N44" s="57"/>
       <c r="O44" s="10">
         <v>6</v>
       </c>
@@ -42082,23 +42082,23 @@
       <c r="AMJ44"/>
     </row>
     <row r="45" spans="1:1254" s="4" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="62" t="s">
-        <v>81</v>
+      <c r="A45" s="61" t="s">
+        <v>80</v>
       </c>
-      <c r="B45" s="62"/>
-      <c r="C45" s="62"/>
-      <c r="D45" s="62"/>
-      <c r="E45" s="62"/>
-      <c r="F45" s="62"/>
-      <c r="G45" s="62"/>
-      <c r="H45" s="62"/>
-      <c r="I45" s="62"/>
-      <c r="J45" s="62"/>
-      <c r="K45" s="62"/>
-      <c r="L45" s="62"/>
-      <c r="M45" s="62"/>
-      <c r="N45" s="62"/>
-      <c r="O45" s="62"/>
+      <c r="B45" s="61"/>
+      <c r="C45" s="61"/>
+      <c r="D45" s="61"/>
+      <c r="E45" s="61"/>
+      <c r="F45" s="61"/>
+      <c r="G45" s="61"/>
+      <c r="H45" s="61"/>
+      <c r="I45" s="61"/>
+      <c r="J45" s="61"/>
+      <c r="K45" s="61"/>
+      <c r="L45" s="61"/>
+      <c r="M45" s="61"/>
+      <c r="N45" s="61"/>
+      <c r="O45" s="61"/>
       <c r="P45"/>
       <c r="Q45"/>
       <c r="R45"/>
@@ -43341,7 +43341,7 @@
     </row>
     <row r="46" spans="1:1254" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B46" s="15">
         <v>13.54</v>
@@ -43354,24 +43354,24 @@
         <v>13.54</v>
       </c>
       <c r="E46" s="20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F46" s="20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G46" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H46" s="55" t="s">
-        <v>142</v>
+      <c r="H46" s="49" t="s">
+        <v>141</v>
       </c>
       <c r="I46" s="36"/>
-      <c r="J46" s="48"/>
-      <c r="K46" s="48"/>
-      <c r="L46" s="48"/>
-      <c r="M46" s="48"/>
-      <c r="N46" s="48"/>
-      <c r="O46" s="48"/>
+      <c r="J46" s="58"/>
+      <c r="K46" s="58"/>
+      <c r="L46" s="58"/>
+      <c r="M46" s="58"/>
+      <c r="N46" s="58"/>
+      <c r="O46" s="58"/>
       <c r="FS46"/>
       <c r="FT46"/>
       <c r="FU46"/>
@@ -44225,7 +44225,7 @@
     </row>
     <row r="47" spans="1:1254" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="27" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B47" s="14">
         <v>10.57</v>
@@ -44241,21 +44241,21 @@
         <v>19</v>
       </c>
       <c r="F47" s="30" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G47" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H47" s="55" t="s">
-        <v>142</v>
+      <c r="H47" s="49" t="s">
+        <v>141</v>
       </c>
       <c r="I47" s="37"/>
-      <c r="J47" s="50"/>
-      <c r="K47" s="50"/>
-      <c r="L47" s="50"/>
-      <c r="M47" s="50"/>
-      <c r="N47" s="50"/>
-      <c r="O47" s="50"/>
+      <c r="J47" s="59"/>
+      <c r="K47" s="59"/>
+      <c r="L47" s="59"/>
+      <c r="M47" s="59"/>
+      <c r="N47" s="59"/>
+      <c r="O47" s="59"/>
       <c r="FS47"/>
       <c r="FT47"/>
       <c r="FU47"/>
@@ -45109,7 +45109,7 @@
     </row>
     <row r="48" spans="1:1254" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="38" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B48" s="14">
         <v>73.180000000000007</v>
@@ -45122,26 +45122,26 @@
         <v>73.180000000000007</v>
       </c>
       <c r="E48" s="30" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F48" s="30" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G48" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H48" s="55" t="s">
-        <v>142</v>
+      <c r="H48" s="49" t="s">
+        <v>141</v>
       </c>
       <c r="I48" s="37"/>
-      <c r="J48" s="48" t="s">
-        <v>90</v>
+      <c r="J48" s="58" t="s">
+        <v>89</v>
       </c>
-      <c r="K48" s="48"/>
-      <c r="L48" s="48"/>
-      <c r="M48" s="48"/>
-      <c r="N48" s="48"/>
-      <c r="O48" s="48"/>
+      <c r="K48" s="58"/>
+      <c r="L48" s="58"/>
+      <c r="M48" s="58"/>
+      <c r="N48" s="58"/>
+      <c r="O48" s="58"/>
       <c r="FS48"/>
       <c r="FT48"/>
       <c r="FU48"/>
@@ -45995,7 +45995,7 @@
     </row>
     <row r="49" spans="1:1254" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="38" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B49" s="14">
         <v>17.399999999999999</v>
@@ -46011,23 +46011,23 @@
         <v>19</v>
       </c>
       <c r="F49" s="30" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G49" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H49" s="55" t="s">
-        <v>142</v>
+      <c r="H49" s="49" t="s">
+        <v>141</v>
       </c>
       <c r="I49" s="34"/>
-      <c r="J49" s="48" t="s">
-        <v>91</v>
+      <c r="J49" s="58" t="s">
+        <v>90</v>
       </c>
-      <c r="K49" s="48"/>
-      <c r="L49" s="48"/>
-      <c r="M49" s="48"/>
-      <c r="N49" s="48"/>
-      <c r="O49" s="48"/>
+      <c r="K49" s="58"/>
+      <c r="L49" s="58"/>
+      <c r="M49" s="58"/>
+      <c r="N49" s="58"/>
+      <c r="O49" s="58"/>
       <c r="FS49"/>
       <c r="FT49"/>
       <c r="FU49"/>
@@ -46881,7 +46881,7 @@
     </row>
     <row r="50" spans="1:1254" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="27" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B50" s="14">
         <v>2.54</v>
@@ -46897,21 +46897,21 @@
         <v>19</v>
       </c>
       <c r="F50" s="30" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G50" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H50" s="55" t="s">
-        <v>142</v>
+      <c r="H50" s="49" t="s">
+        <v>141</v>
       </c>
       <c r="I50" s="34"/>
-      <c r="J50" s="48"/>
-      <c r="K50" s="48"/>
-      <c r="L50" s="48"/>
-      <c r="M50" s="48"/>
-      <c r="N50" s="48"/>
-      <c r="O50" s="48"/>
+      <c r="J50" s="58"/>
+      <c r="K50" s="58"/>
+      <c r="L50" s="58"/>
+      <c r="M50" s="58"/>
+      <c r="N50" s="58"/>
+      <c r="O50" s="58"/>
       <c r="FS50"/>
       <c r="FT50"/>
       <c r="FU50"/>
@@ -47765,7 +47765,7 @@
     </row>
     <row r="51" spans="1:1254" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="38" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B51" s="14">
         <v>18.95</v>
@@ -47778,26 +47778,26 @@
         <v>18.95</v>
       </c>
       <c r="E51" s="30" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F51" s="30" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G51" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H51" s="55" t="s">
-        <v>142</v>
+      <c r="H51" s="49" t="s">
+        <v>141</v>
       </c>
       <c r="I51" s="34"/>
-      <c r="J51" s="48" t="s">
-        <v>96</v>
+      <c r="J51" s="58" t="s">
+        <v>95</v>
       </c>
-      <c r="K51" s="48"/>
-      <c r="L51" s="48"/>
-      <c r="M51" s="48"/>
-      <c r="N51" s="48"/>
-      <c r="O51" s="48"/>
+      <c r="K51" s="58"/>
+      <c r="L51" s="58"/>
+      <c r="M51" s="58"/>
+      <c r="N51" s="58"/>
+      <c r="O51" s="58"/>
       <c r="FS51"/>
       <c r="FT51"/>
       <c r="FU51"/>
@@ -48651,7 +48651,7 @@
     </row>
     <row r="52" spans="1:1254" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="38" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B52" s="14">
         <v>73.180000000000007</v>
@@ -48664,24 +48664,24 @@
         <v>73.180000000000007</v>
       </c>
       <c r="E52" s="30" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F52" s="30" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G52" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H52" s="55" t="s">
-        <v>142</v>
+      <c r="H52" s="49" t="s">
+        <v>141</v>
       </c>
       <c r="I52" s="37"/>
-      <c r="J52" s="48"/>
-      <c r="K52" s="48"/>
-      <c r="L52" s="48"/>
-      <c r="M52" s="48"/>
-      <c r="N52" s="48"/>
-      <c r="O52" s="48"/>
+      <c r="J52" s="58"/>
+      <c r="K52" s="58"/>
+      <c r="L52" s="58"/>
+      <c r="M52" s="58"/>
+      <c r="N52" s="58"/>
+      <c r="O52" s="58"/>
       <c r="FS52"/>
       <c r="FT52"/>
       <c r="FU52"/>
@@ -49535,7 +49535,7 @@
     </row>
     <row r="53" spans="1:1254" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="27" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B53" s="14">
         <v>2.81</v>
@@ -49551,21 +49551,21 @@
         <v>19</v>
       </c>
       <c r="F53" s="30" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G53" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H53" s="55" t="s">
-        <v>142</v>
+      <c r="H53" s="49" t="s">
+        <v>141</v>
       </c>
       <c r="I53" s="34"/>
-      <c r="J53" s="48"/>
-      <c r="K53" s="48"/>
-      <c r="L53" s="48"/>
-      <c r="M53" s="48"/>
-      <c r="N53" s="48"/>
-      <c r="O53" s="48"/>
+      <c r="J53" s="58"/>
+      <c r="K53" s="58"/>
+      <c r="L53" s="58"/>
+      <c r="M53" s="58"/>
+      <c r="N53" s="58"/>
+      <c r="O53" s="58"/>
       <c r="FS53"/>
       <c r="FT53"/>
       <c r="FU53"/>
@@ -50419,7 +50419,7 @@
     </row>
     <row r="54" spans="1:1254" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="27" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B54" s="14">
         <v>3.69</v>
@@ -50435,21 +50435,21 @@
         <v>19</v>
       </c>
       <c r="F54" s="30" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G54" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H54" s="55" t="s">
-        <v>142</v>
+      <c r="H54" s="49" t="s">
+        <v>141</v>
       </c>
       <c r="I54" s="34"/>
-      <c r="J54" s="48"/>
-      <c r="K54" s="48"/>
-      <c r="L54" s="48"/>
-      <c r="M54" s="48"/>
-      <c r="N54" s="48"/>
-      <c r="O54" s="48"/>
+      <c r="J54" s="58"/>
+      <c r="K54" s="58"/>
+      <c r="L54" s="58"/>
+      <c r="M54" s="58"/>
+      <c r="N54" s="58"/>
+      <c r="O54" s="58"/>
       <c r="FS54"/>
       <c r="FT54"/>
       <c r="FU54"/>
@@ -51303,7 +51303,7 @@
     </row>
     <row r="55" spans="1:1254" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="27" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B55" s="14">
         <v>15.32</v>
@@ -51316,26 +51316,26 @@
         <v>15.32</v>
       </c>
       <c r="E55" s="30" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F55" s="39" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G55" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H55" s="55" t="s">
-        <v>142</v>
+      <c r="H55" s="49" t="s">
+        <v>141</v>
       </c>
       <c r="I55" s="34"/>
-      <c r="J55" s="48" t="s">
-        <v>105</v>
+      <c r="J55" s="58" t="s">
+        <v>104</v>
       </c>
-      <c r="K55" s="48"/>
-      <c r="L55" s="48"/>
-      <c r="M55" s="48"/>
-      <c r="N55" s="48"/>
-      <c r="O55" s="48"/>
+      <c r="K55" s="58"/>
+      <c r="L55" s="58"/>
+      <c r="M55" s="58"/>
+      <c r="N55" s="58"/>
+      <c r="O55" s="58"/>
       <c r="FS55"/>
       <c r="FT55"/>
       <c r="FU55"/>
@@ -52189,7 +52189,7 @@
     </row>
     <row r="56" spans="1:1254" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="27" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B56" s="14">
         <v>56.31</v>
@@ -52202,26 +52202,26 @@
         <v>56.31</v>
       </c>
       <c r="E56" s="30" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F56" s="30" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G56" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H56" s="55" t="s">
-        <v>142</v>
+      <c r="H56" s="49" t="s">
+        <v>141</v>
       </c>
       <c r="I56" s="34"/>
-      <c r="J56" s="48" t="s">
-        <v>106</v>
+      <c r="J56" s="58" t="s">
+        <v>105</v>
       </c>
-      <c r="K56" s="48"/>
-      <c r="L56" s="48"/>
-      <c r="M56" s="48"/>
-      <c r="N56" s="48"/>
-      <c r="O56" s="48"/>
+      <c r="K56" s="58"/>
+      <c r="L56" s="58"/>
+      <c r="M56" s="58"/>
+      <c r="N56" s="58"/>
+      <c r="O56" s="58"/>
       <c r="FS56"/>
       <c r="FT56"/>
       <c r="FU56"/>
@@ -53075,7 +53075,7 @@
     </row>
     <row r="57" spans="1:1254" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="38" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B57" s="14">
         <v>17.399999999999999</v>
@@ -53091,21 +53091,21 @@
         <v>19</v>
       </c>
       <c r="F57" s="30" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G57" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H57" s="55" t="s">
-        <v>142</v>
+      <c r="H57" s="49" t="s">
+        <v>141</v>
       </c>
       <c r="I57" s="34"/>
-      <c r="J57" s="48"/>
-      <c r="K57" s="48"/>
-      <c r="L57" s="48"/>
-      <c r="M57" s="48"/>
-      <c r="N57" s="48"/>
-      <c r="O57" s="48"/>
+      <c r="J57" s="58"/>
+      <c r="K57" s="58"/>
+      <c r="L57" s="58"/>
+      <c r="M57" s="58"/>
+      <c r="N57" s="58"/>
+      <c r="O57" s="58"/>
       <c r="FS57"/>
       <c r="FT57"/>
       <c r="FU57"/>
@@ -53959,7 +53959,7 @@
     </row>
     <row r="58" spans="1:1254" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="27" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B58" s="14">
         <v>66.39</v>
@@ -53975,21 +53975,21 @@
         <v>19</v>
       </c>
       <c r="F58" s="30" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G58" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H58" s="55" t="s">
-        <v>142</v>
+      <c r="H58" s="49" t="s">
+        <v>141</v>
       </c>
       <c r="I58" s="34"/>
-      <c r="J58" s="48"/>
-      <c r="K58" s="48"/>
-      <c r="L58" s="48"/>
-      <c r="M58" s="48"/>
-      <c r="N58" s="48"/>
-      <c r="O58" s="48"/>
+      <c r="J58" s="58"/>
+      <c r="K58" s="58"/>
+      <c r="L58" s="58"/>
+      <c r="M58" s="58"/>
+      <c r="N58" s="58"/>
+      <c r="O58" s="58"/>
       <c r="FS58"/>
       <c r="FT58"/>
       <c r="FU58"/>
@@ -54843,7 +54843,7 @@
     </row>
     <row r="59" spans="1:1254" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="27" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B59" s="14">
         <v>16.98</v>
@@ -54856,24 +54856,24 @@
         <v>33.96</v>
       </c>
       <c r="E59" s="30" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F59" s="30" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G59" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H59" s="55" t="s">
-        <v>142</v>
+      <c r="H59" s="49" t="s">
+        <v>141</v>
       </c>
       <c r="I59" s="34"/>
-      <c r="J59" s="48"/>
-      <c r="K59" s="48"/>
-      <c r="L59" s="48"/>
-      <c r="M59" s="48"/>
-      <c r="N59" s="48"/>
-      <c r="O59" s="48"/>
+      <c r="J59" s="58"/>
+      <c r="K59" s="58"/>
+      <c r="L59" s="58"/>
+      <c r="M59" s="58"/>
+      <c r="N59" s="58"/>
+      <c r="O59" s="58"/>
       <c r="FS59"/>
       <c r="FT59"/>
       <c r="FU59"/>
@@ -55727,7 +55727,7 @@
     </row>
     <row r="60" spans="1:1254" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="38" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B60" s="14">
         <v>24.85</v>
@@ -55743,21 +55743,21 @@
         <v>19</v>
       </c>
       <c r="F60" s="30" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G60" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H60" s="55" t="s">
-        <v>142</v>
+      <c r="H60" s="49" t="s">
+        <v>141</v>
       </c>
       <c r="I60" s="34"/>
-      <c r="J60" s="48"/>
-      <c r="K60" s="48"/>
-      <c r="L60" s="48"/>
-      <c r="M60" s="48"/>
-      <c r="N60" s="48"/>
-      <c r="O60" s="48"/>
+      <c r="J60" s="58"/>
+      <c r="K60" s="58"/>
+      <c r="L60" s="58"/>
+      <c r="M60" s="58"/>
+      <c r="N60" s="58"/>
+      <c r="O60" s="58"/>
       <c r="FS60"/>
       <c r="FT60"/>
       <c r="FU60"/>
@@ -56611,7 +56611,7 @@
     </row>
     <row r="61" spans="1:1254" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="38" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B61" s="14">
         <v>16.2</v>
@@ -56627,21 +56627,21 @@
         <v>19</v>
       </c>
       <c r="F61" s="30" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G61" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H61" s="55" t="s">
-        <v>142</v>
+      <c r="H61" s="49" t="s">
+        <v>141</v>
       </c>
       <c r="I61" s="34"/>
-      <c r="J61" s="48"/>
-      <c r="K61" s="48"/>
-      <c r="L61" s="48"/>
-      <c r="M61" s="48"/>
-      <c r="N61" s="48"/>
-      <c r="O61" s="48"/>
+      <c r="J61" s="58"/>
+      <c r="K61" s="58"/>
+      <c r="L61" s="58"/>
+      <c r="M61" s="58"/>
+      <c r="N61" s="58"/>
+      <c r="O61" s="58"/>
       <c r="FS61"/>
       <c r="FT61"/>
       <c r="FU61"/>
@@ -57495,7 +57495,7 @@
     </row>
     <row r="62" spans="1:1254" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="27" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B62" s="14">
         <v>49.39</v>
@@ -57511,21 +57511,21 @@
         <v>19</v>
       </c>
       <c r="F62" s="30" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G62" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H62" s="55" t="s">
-        <v>142</v>
+      <c r="H62" s="49" t="s">
+        <v>141</v>
       </c>
       <c r="I62" s="34"/>
-      <c r="J62" s="48"/>
-      <c r="K62" s="48"/>
-      <c r="L62" s="48"/>
-      <c r="M62" s="48"/>
-      <c r="N62" s="48"/>
-      <c r="O62" s="48"/>
+      <c r="J62" s="58"/>
+      <c r="K62" s="58"/>
+      <c r="L62" s="58"/>
+      <c r="M62" s="58"/>
+      <c r="N62" s="58"/>
+      <c r="O62" s="58"/>
       <c r="FS62"/>
       <c r="FT62"/>
       <c r="FU62"/>
@@ -58379,7 +58379,7 @@
     </row>
     <row r="63" spans="1:1254" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="27" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B63" s="14">
         <v>131.82</v>
@@ -58392,24 +58392,24 @@
         <v>131.82</v>
       </c>
       <c r="E63" s="30" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F63" s="30" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G63" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H63" s="55" t="s">
-        <v>142</v>
+      <c r="H63" s="49" t="s">
+        <v>141</v>
       </c>
       <c r="I63" s="34"/>
-      <c r="J63" s="48"/>
-      <c r="K63" s="48"/>
-      <c r="L63" s="48"/>
-      <c r="M63" s="48"/>
-      <c r="N63" s="48"/>
-      <c r="O63" s="48"/>
+      <c r="J63" s="58"/>
+      <c r="K63" s="58"/>
+      <c r="L63" s="58"/>
+      <c r="M63" s="58"/>
+      <c r="N63" s="58"/>
+      <c r="O63" s="58"/>
       <c r="FS63"/>
       <c r="FT63"/>
       <c r="FU63"/>
@@ -59262,23 +59262,23 @@
       <c r="AMJ63"/>
     </row>
     <row r="64" spans="1:1254" s="4" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="62" t="s">
-        <v>71</v>
+      <c r="A64" s="61" t="s">
+        <v>70</v>
       </c>
-      <c r="B64" s="62"/>
-      <c r="C64" s="62"/>
-      <c r="D64" s="62"/>
-      <c r="E64" s="62"/>
-      <c r="F64" s="62"/>
-      <c r="G64" s="62"/>
-      <c r="H64" s="62"/>
-      <c r="I64" s="62"/>
-      <c r="J64" s="62"/>
-      <c r="K64" s="62"/>
-      <c r="L64" s="62"/>
-      <c r="M64" s="62"/>
-      <c r="N64" s="62"/>
-      <c r="O64" s="62"/>
+      <c r="B64" s="61"/>
+      <c r="C64" s="61"/>
+      <c r="D64" s="61"/>
+      <c r="E64" s="61"/>
+      <c r="F64" s="61"/>
+      <c r="G64" s="61"/>
+      <c r="H64" s="61"/>
+      <c r="I64" s="61"/>
+      <c r="J64" s="61"/>
+      <c r="K64" s="61"/>
+      <c r="L64" s="61"/>
+      <c r="M64" s="61"/>
+      <c r="N64" s="61"/>
+      <c r="O64" s="61"/>
       <c r="P64"/>
       <c r="Q64"/>
       <c r="R64"/>
@@ -60531,12 +60531,12 @@
       </c>
       <c r="H65" s="44"/>
       <c r="I65" s="40"/>
-      <c r="J65" s="52"/>
-      <c r="K65" s="52"/>
-      <c r="L65" s="52"/>
-      <c r="M65" s="52"/>
-      <c r="N65" s="52"/>
-      <c r="O65" s="52"/>
+      <c r="J65" s="60"/>
+      <c r="K65" s="60"/>
+      <c r="L65" s="60"/>
+      <c r="M65" s="60"/>
+      <c r="N65" s="60"/>
+      <c r="O65" s="60"/>
       <c r="P65"/>
       <c r="Q65"/>
       <c r="R65"/>
@@ -61789,12 +61789,12 @@
       </c>
       <c r="H66" s="44"/>
       <c r="I66" s="40"/>
-      <c r="J66" s="52"/>
-      <c r="K66" s="52"/>
-      <c r="L66" s="52"/>
-      <c r="M66" s="52"/>
-      <c r="N66" s="52"/>
-      <c r="O66" s="52"/>
+      <c r="J66" s="60"/>
+      <c r="K66" s="60"/>
+      <c r="L66" s="60"/>
+      <c r="M66" s="60"/>
+      <c r="N66" s="60"/>
+      <c r="O66" s="60"/>
       <c r="P66"/>
       <c r="Q66"/>
       <c r="R66"/>
@@ -63036,23 +63036,23 @@
       <c r="AVF66"/>
     </row>
     <row r="67" spans="1:1254" ht="19.350000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="62" t="s">
-        <v>72</v>
+      <c r="A67" s="61" t="s">
+        <v>71</v>
       </c>
-      <c r="B67" s="62"/>
-      <c r="C67" s="62"/>
-      <c r="D67" s="62"/>
-      <c r="E67" s="62"/>
-      <c r="F67" s="62"/>
-      <c r="G67" s="62"/>
-      <c r="H67" s="62"/>
-      <c r="I67" s="62"/>
-      <c r="J67" s="62"/>
-      <c r="K67" s="62"/>
-      <c r="L67" s="62"/>
-      <c r="M67" s="62"/>
-      <c r="N67" s="62"/>
-      <c r="O67" s="62"/>
+      <c r="B67" s="61"/>
+      <c r="C67" s="61"/>
+      <c r="D67" s="61"/>
+      <c r="E67" s="61"/>
+      <c r="F67" s="61"/>
+      <c r="G67" s="61"/>
+      <c r="H67" s="61"/>
+      <c r="I67" s="61"/>
+      <c r="J67" s="61"/>
+      <c r="K67" s="61"/>
+      <c r="L67" s="61"/>
+      <c r="M67" s="61"/>
+      <c r="N67" s="61"/>
+      <c r="O67" s="61"/>
       <c r="FS67"/>
       <c r="FT67"/>
       <c r="FU67"/>
@@ -63906,7 +63906,7 @@
     </row>
     <row r="68" spans="1:1254" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="45" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B68" s="13">
         <v>28.8</v>
@@ -63919,24 +63919,24 @@
         <v>28.8</v>
       </c>
       <c r="E68" s="46" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F68" s="23" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G68" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H68" s="55" t="s">
-        <v>142</v>
+      <c r="H68" s="49" t="s">
+        <v>141</v>
       </c>
       <c r="I68" s="47"/>
-      <c r="J68" s="50"/>
-      <c r="K68" s="50"/>
-      <c r="L68" s="50"/>
-      <c r="M68" s="50"/>
-      <c r="N68" s="50"/>
-      <c r="O68" s="50"/>
+      <c r="J68" s="59"/>
+      <c r="K68" s="59"/>
+      <c r="L68" s="59"/>
+      <c r="M68" s="59"/>
+      <c r="N68" s="59"/>
+      <c r="O68" s="59"/>
       <c r="FS68"/>
       <c r="FT68"/>
       <c r="FU68"/>
@@ -64790,7 +64790,7 @@
     </row>
     <row r="69" spans="1:1254" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="27" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B69" s="14">
         <v>20.25</v>
@@ -64806,23 +64806,23 @@
         <v>19</v>
       </c>
       <c r="F69" s="30" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G69" s="28" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
-      <c r="H69" s="55" t="s">
-        <v>142</v>
+      <c r="H69" s="49" t="s">
+        <v>141</v>
       </c>
       <c r="I69" s="34"/>
-      <c r="J69" s="50" t="s">
-        <v>119</v>
+      <c r="J69" s="59" t="s">
+        <v>118</v>
       </c>
-      <c r="K69" s="50"/>
-      <c r="L69" s="50"/>
-      <c r="M69" s="50"/>
-      <c r="N69" s="50"/>
-      <c r="O69" s="50"/>
+      <c r="K69" s="59"/>
+      <c r="L69" s="59"/>
+      <c r="M69" s="59"/>
+      <c r="N69" s="59"/>
+      <c r="O69" s="59"/>
       <c r="FS69"/>
       <c r="FT69"/>
       <c r="FU69"/>
@@ -65676,7 +65676,7 @@
     </row>
     <row r="70" spans="1:1254" s="4" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="27" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B70" s="14">
         <v>2.63</v>
@@ -65692,23 +65692,23 @@
         <v>19</v>
       </c>
       <c r="F70" s="30" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G70" s="28" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
-      <c r="H70" s="55" t="s">
-        <v>142</v>
+      <c r="H70" s="49" t="s">
+        <v>141</v>
       </c>
       <c r="I70" s="34"/>
-      <c r="J70" s="50" t="s">
-        <v>120</v>
+      <c r="J70" s="59" t="s">
+        <v>119</v>
       </c>
-      <c r="K70" s="50"/>
-      <c r="L70" s="50"/>
-      <c r="M70" s="50"/>
-      <c r="N70" s="50"/>
-      <c r="O70" s="50"/>
+      <c r="K70" s="59"/>
+      <c r="L70" s="59"/>
+      <c r="M70" s="59"/>
+      <c r="N70" s="59"/>
+      <c r="O70" s="59"/>
       <c r="P70"/>
       <c r="Q70"/>
       <c r="R70"/>
@@ -66950,12 +66950,12 @@
       <c r="AVF70"/>
     </row>
     <row r="71" spans="1:1254" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="58" t="s">
-        <v>130</v>
+      <c r="A71" s="54" t="s">
+        <v>129</v>
       </c>
-      <c r="B71" s="59"/>
-      <c r="C71" s="60"/>
-      <c r="D71" s="61">
+      <c r="B71" s="55"/>
+      <c r="C71" s="56"/>
+      <c r="D71" s="52">
         <f>SUM(D3:D5,D7:D21,D23:D28,D30:D35,D37:D42,D46:D63,D68:D70)</f>
         <v>2120.8760000000002</v>
       </c>
@@ -69527,15 +69527,52 @@
     </row>
   </sheetData>
   <mergeCells count="71">
-    <mergeCell ref="A71:C71"/>
-    <mergeCell ref="J37:N37"/>
-    <mergeCell ref="J41:N41"/>
-    <mergeCell ref="J40:N40"/>
-    <mergeCell ref="J39:N39"/>
-    <mergeCell ref="J38:N38"/>
-    <mergeCell ref="J44:N44"/>
-    <mergeCell ref="J43:N43"/>
-    <mergeCell ref="J42:N42"/>
+    <mergeCell ref="J30:O30"/>
+    <mergeCell ref="J31:O31"/>
+    <mergeCell ref="A29:O29"/>
+    <mergeCell ref="J68:O68"/>
+    <mergeCell ref="A36:O36"/>
+    <mergeCell ref="J62:O62"/>
+    <mergeCell ref="J57:O57"/>
+    <mergeCell ref="J56:O56"/>
+    <mergeCell ref="J55:O55"/>
+    <mergeCell ref="J54:O54"/>
+    <mergeCell ref="J53:O53"/>
+    <mergeCell ref="J46:O46"/>
+    <mergeCell ref="J48:O48"/>
+    <mergeCell ref="J24:O24"/>
+    <mergeCell ref="J25:O25"/>
+    <mergeCell ref="A22:O22"/>
+    <mergeCell ref="J21:O21"/>
+    <mergeCell ref="J63:O63"/>
+    <mergeCell ref="J32:O32"/>
+    <mergeCell ref="J33:O33"/>
+    <mergeCell ref="J34:O34"/>
+    <mergeCell ref="J35:O35"/>
+    <mergeCell ref="J49:O49"/>
+    <mergeCell ref="J59:O59"/>
+    <mergeCell ref="J58:O58"/>
+    <mergeCell ref="J61:O61"/>
+    <mergeCell ref="J60:O60"/>
+    <mergeCell ref="J26:O26"/>
+    <mergeCell ref="J27:O27"/>
+    <mergeCell ref="J16:O16"/>
+    <mergeCell ref="J17:O17"/>
+    <mergeCell ref="J18:O18"/>
+    <mergeCell ref="J19:O19"/>
+    <mergeCell ref="J23:O23"/>
+    <mergeCell ref="J1:O1"/>
+    <mergeCell ref="J3:O3"/>
+    <mergeCell ref="J4:O4"/>
+    <mergeCell ref="J5:O5"/>
+    <mergeCell ref="J7:O7"/>
+    <mergeCell ref="A6:O6"/>
+    <mergeCell ref="A2:O2"/>
+    <mergeCell ref="J8:O8"/>
+    <mergeCell ref="J9:O9"/>
+    <mergeCell ref="J10:O10"/>
+    <mergeCell ref="J11:O11"/>
+    <mergeCell ref="J12:O12"/>
     <mergeCell ref="J13:O13"/>
     <mergeCell ref="J14:O14"/>
     <mergeCell ref="J70:O70"/>
@@ -69552,52 +69589,15 @@
     <mergeCell ref="J50:O50"/>
     <mergeCell ref="J47:O47"/>
     <mergeCell ref="J15:O15"/>
-    <mergeCell ref="J8:O8"/>
-    <mergeCell ref="J9:O9"/>
-    <mergeCell ref="J10:O10"/>
-    <mergeCell ref="J11:O11"/>
-    <mergeCell ref="J12:O12"/>
-    <mergeCell ref="J1:O1"/>
-    <mergeCell ref="J3:O3"/>
-    <mergeCell ref="J4:O4"/>
-    <mergeCell ref="J5:O5"/>
-    <mergeCell ref="J7:O7"/>
-    <mergeCell ref="A6:O6"/>
-    <mergeCell ref="A2:O2"/>
-    <mergeCell ref="J16:O16"/>
-    <mergeCell ref="J17:O17"/>
-    <mergeCell ref="J18:O18"/>
-    <mergeCell ref="J19:O19"/>
-    <mergeCell ref="J23:O23"/>
-    <mergeCell ref="J24:O24"/>
-    <mergeCell ref="J25:O25"/>
-    <mergeCell ref="A22:O22"/>
-    <mergeCell ref="J21:O21"/>
-    <mergeCell ref="J63:O63"/>
-    <mergeCell ref="J32:O32"/>
-    <mergeCell ref="J33:O33"/>
-    <mergeCell ref="J34:O34"/>
-    <mergeCell ref="J35:O35"/>
-    <mergeCell ref="J49:O49"/>
-    <mergeCell ref="J59:O59"/>
-    <mergeCell ref="J58:O58"/>
-    <mergeCell ref="J61:O61"/>
-    <mergeCell ref="J60:O60"/>
-    <mergeCell ref="J26:O26"/>
-    <mergeCell ref="J27:O27"/>
-    <mergeCell ref="J30:O30"/>
-    <mergeCell ref="J31:O31"/>
-    <mergeCell ref="A29:O29"/>
-    <mergeCell ref="J68:O68"/>
-    <mergeCell ref="A36:O36"/>
-    <mergeCell ref="J62:O62"/>
-    <mergeCell ref="J57:O57"/>
-    <mergeCell ref="J56:O56"/>
-    <mergeCell ref="J55:O55"/>
-    <mergeCell ref="J54:O54"/>
-    <mergeCell ref="J53:O53"/>
-    <mergeCell ref="J46:O46"/>
-    <mergeCell ref="J48:O48"/>
+    <mergeCell ref="A71:C71"/>
+    <mergeCell ref="J37:N37"/>
+    <mergeCell ref="J41:N41"/>
+    <mergeCell ref="J40:N40"/>
+    <mergeCell ref="J39:N39"/>
+    <mergeCell ref="J38:N38"/>
+    <mergeCell ref="J44:N44"/>
+    <mergeCell ref="J43:N43"/>
+    <mergeCell ref="J42:N42"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="H7" r:id="rId1" location="90967A160" tooltip="LINK"/>

</xml_diff>